<commit_message>
adding more updates to example rtm
</commit_message>
<xml_diff>
--- a/Project 1/Example RTM.xlsx
+++ b/Project 1/Example RTM.xlsx
@@ -8,16 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EricSuminski\Desktop\241209-JWA\Project 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5984AA7-C5CA-4D5F-A590-EB0B3658E6E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69881355-B43D-40F0-934F-13E14A83F31B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" firstSheet="1" activeTab="4" xr2:uid="{F782749A-F44B-4770-ADC0-B107849E38C9}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" firstSheet="1" activeTab="1" xr2:uid="{F782749A-F44B-4770-ADC0-B107849E38C9}"/>
   </bookViews>
   <sheets>
     <sheet name="User Stories" sheetId="1" r:id="rId1"/>
-    <sheet name="Security Requirements" sheetId="2" r:id="rId2"/>
-    <sheet name="User Requirements" sheetId="3" r:id="rId3"/>
-    <sheet name="Planet Requirements" sheetId="4" r:id="rId4"/>
-    <sheet name="Moon Requirements" sheetId="5" r:id="rId5"/>
+    <sheet name="Mapping" sheetId="6" r:id="rId2"/>
+    <sheet name="Security Requirements" sheetId="2" r:id="rId3"/>
+    <sheet name="User Requirements" sheetId="3" r:id="rId4"/>
+    <sheet name="Planet Requirements" sheetId="4" r:id="rId5"/>
+    <sheet name="Moon Requirements" sheetId="5" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="61">
   <si>
     <t>ID</t>
   </si>
@@ -78,12 +79,6 @@
     <t>US5</t>
   </si>
   <si>
-    <t>Column1</t>
-  </si>
-  <si>
-    <t>Column2</t>
-  </si>
-  <si>
     <t>Security Requirement</t>
   </si>
   <si>
@@ -223,6 +218,12 @@
   </si>
   <si>
     <t>MR7</t>
+  </si>
+  <si>
+    <t>Requirement</t>
+  </si>
+  <si>
+    <t>To Be Continued!</t>
   </si>
 </sst>
 </file>
@@ -258,16 +259,22 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="20">
+  <dxfs count="21">
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -342,55 +349,66 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7A75172B-577E-4D84-AF49-87F5C4778595}" name="Table1" displayName="Table1" ref="A1:B7" totalsRowShown="0" headerRowDxfId="16" dataDxfId="17">
-  <autoFilter ref="A1:B7" xr:uid="{7A75172B-577E-4D84-AF49-87F5C4778595}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7A75172B-577E-4D84-AF49-87F5C4778595}" name="Table1" displayName="Table1" ref="A1:B6" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
+  <autoFilter ref="A1:B6" xr:uid="{7A75172B-577E-4D84-AF49-87F5C4778595}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{FED0608C-55BC-4321-8720-E641D878198E}" name="Column1" dataDxfId="19"/>
-    <tableColumn id="2" xr3:uid="{5B7B44D4-81F7-4CA6-98CC-2C160723D4F2}" name="Column2" dataDxfId="18"/>
+    <tableColumn id="1" xr3:uid="{FED0608C-55BC-4321-8720-E641D878198E}" name="ID" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{5B7B44D4-81F7-4CA6-98CC-2C160723D4F2}" name="User Story" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{CF32EC7D-69C5-4A93-8A2D-DC6765B2E759}" name="Table2" displayName="Table2" ref="A1:B5" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12">
-  <autoFilter ref="A1:B5" xr:uid="{CF32EC7D-69C5-4A93-8A2D-DC6765B2E759}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{8C7A2EF1-1E3B-497A-963A-1E4B297B1AD8}" name="Table6" displayName="Table6" ref="A1:B11" totalsRowShown="0" headerRowDxfId="0">
+  <autoFilter ref="A1:B11" xr:uid="{8C7A2EF1-1E3B-497A-963A-1E4B297B1AD8}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{516DE414-3CB5-42C3-B197-5FD33F813523}" name="Column1" dataDxfId="15"/>
-    <tableColumn id="2" xr3:uid="{6D770425-64E8-434C-8D03-6414A09F53EC}" name="Column2" dataDxfId="14"/>
+    <tableColumn id="1" xr3:uid="{3E1D6F9B-CF49-4C23-A4F1-14FC88593279}" name="User Story"/>
+    <tableColumn id="2" xr3:uid="{0AE99736-D95C-4721-996D-FB61185AF45C}" name="Requirement"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleDark5" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{CF32EC7D-69C5-4A93-8A2D-DC6765B2E759}" name="Table2" displayName="Table2" ref="A1:B4" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
+  <autoFilter ref="A1:B4" xr:uid="{CF32EC7D-69C5-4A93-8A2D-DC6765B2E759}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{516DE414-3CB5-42C3-B197-5FD33F813523}" name="ID" dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{6D770425-64E8-434C-8D03-6414A09F53EC}" name="Security Requirement" dataDxfId="5"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
-<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{402AD37E-496A-4B82-BD5A-DDA158D6DA5D}" name="Table3" displayName="Table3" ref="A1:B8" totalsRowShown="0" headerRowDxfId="8" dataDxfId="9">
-  <autoFilter ref="A1:B8" xr:uid="{402AD37E-496A-4B82-BD5A-DDA158D6DA5D}"/>
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{402AD37E-496A-4B82-BD5A-DDA158D6DA5D}" name="Table3" displayName="Table3" ref="A1:B7" totalsRowShown="0" headerRowDxfId="17" dataDxfId="18">
+  <autoFilter ref="A1:B7" xr:uid="{402AD37E-496A-4B82-BD5A-DDA158D6DA5D}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{77E4F913-7B38-4531-8FAA-D16B0FAAB464}" name="Column1" dataDxfId="11"/>
-    <tableColumn id="2" xr3:uid="{85281BD9-33CE-4F6C-84B3-1E17141FF66A}" name="Column2" dataDxfId="10"/>
+    <tableColumn id="1" xr3:uid="{77E4F913-7B38-4531-8FAA-D16B0FAAB464}" name="ID" dataDxfId="20"/>
+    <tableColumn id="2" xr3:uid="{85281BD9-33CE-4F6C-84B3-1E17141FF66A}" name="User Requirement" dataDxfId="19"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
-<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{79042BBB-0F12-4F67-90F0-C8062A2B8101}" name="Table4" displayName="Table4" ref="A1:B8" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
-  <autoFilter ref="A1:B8" xr:uid="{79042BBB-0F12-4F67-90F0-C8062A2B8101}"/>
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{79042BBB-0F12-4F67-90F0-C8062A2B8101}" name="Table4" displayName="Table4" ref="A1:B7" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13">
+  <autoFilter ref="A1:B7" xr:uid="{79042BBB-0F12-4F67-90F0-C8062A2B8101}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{EC350D5A-6EAD-426C-A18A-35EC1B171BC1}" name="Column1" dataDxfId="7"/>
-    <tableColumn id="2" xr3:uid="{690F5785-7E7F-4D6A-8A10-FEEAAFDE3874}" name="Column2" dataDxfId="6"/>
+    <tableColumn id="1" xr3:uid="{EC350D5A-6EAD-426C-A18A-35EC1B171BC1}" name="ID" dataDxfId="16"/>
+    <tableColumn id="2" xr3:uid="{690F5785-7E7F-4D6A-8A10-FEEAAFDE3874}" name="Planet Requirement" dataDxfId="15"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
-<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{CB73B250-B846-4BAF-AF3B-5117DBBA4973}" name="Table5" displayName="Table5" ref="A1:B9" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0">
-  <autoFilter ref="A1:B9" xr:uid="{CB73B250-B846-4BAF-AF3B-5117DBBA4973}"/>
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{CB73B250-B846-4BAF-AF3B-5117DBBA4973}" name="Table5" displayName="Table5" ref="A1:B8" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9">
+  <autoFilter ref="A1:B8" xr:uid="{CB73B250-B846-4BAF-AF3B-5117DBBA4973}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{486EA324-F847-400D-80A5-266D5E36FC20}" name="Column1" dataDxfId="3"/>
-    <tableColumn id="2" xr3:uid="{96D5BDBF-2AB3-4652-A2F0-CF69353F8D08}" name="Column2" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{486EA324-F847-400D-80A5-266D5E36FC20}" name="ID" dataDxfId="12"/>
+    <tableColumn id="2" xr3:uid="{96D5BDBF-2AB3-4652-A2F0-CF69353F8D08}" name="Moon Requirement" dataDxfId="11"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -713,10 +731,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FEED5DBC-B7FC-494C-9A91-44725C18C65A}">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A3" sqref="A3:B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -728,58 +746,50 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
     </row>
+    <row r="2" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
     <row r="3" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>2</v>
+      <c r="A3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>3</v>
+      <c r="A4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>4</v>
+      <c r="A5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+      <c r="A6" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B6" s="2" t="s">
         <v>6</v>
       </c>
     </row>
@@ -792,58 +802,162 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{751CFA12-0342-4856-9D1B-B622A006DBE5}">
+  <dimension ref="A1:B13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.42578125" customWidth="1"/>
+    <col min="2" max="2" width="18.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>60</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4F326BC-F067-41E8-847E-757ABB716A4D}">
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="A4" sqref="A4:B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="27.5703125" customWidth="1"/>
     <col min="2" max="2" width="27.7109375" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="1" t="s">
+    <row r="3" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+    <row r="4" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B4" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>17</v>
-      </c>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -853,12 +967,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34D5955B-CBB4-4821-99BF-DB0B1EC1B1EA}">
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="B2" sqref="B2:B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -869,67 +983,63 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+    <row r="4" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B4" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+    <row r="5" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B5" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+    <row r="6" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B6" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+    <row r="7" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B7" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>27</v>
-      </c>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -939,12 +1049,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46FBBBD4-BA32-4762-983D-1911FDD83C85}">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -954,67 +1064,63 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>0</v>
+        <v>39</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+    <row r="4" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B4" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+    <row r="5" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B5" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+    <row r="6" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B6" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+    <row r="7" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B7" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>40</v>
-      </c>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
@@ -1028,12 +1134,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A2FE8F8-EFC1-44EB-82E1-9A97A755E2C6}">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1044,75 +1150,71 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>0</v>
+        <v>52</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+    <row r="4" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B4" s="1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+    <row r="5" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B5" s="1" t="s">
         <v>49</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B7" s="1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+    <row r="8" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>59</v>
-      </c>
       <c r="B8" s="1" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>40</v>
-      </c>
+        <v>38</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
updating rtm and adding gherkin notes
</commit_message>
<xml_diff>
--- a/Project 1/Example RTM.xlsx
+++ b/Project 1/Example RTM.xlsx
@@ -8,17 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EricSuminski\Desktop\241209-JWA\Project 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69881355-B43D-40F0-934F-13E14A83F31B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D64639A-A73D-426D-A8FF-183510A411CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" firstSheet="1" activeTab="1" xr2:uid="{F782749A-F44B-4770-ADC0-B107849E38C9}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="2" xr2:uid="{F782749A-F44B-4770-ADC0-B107849E38C9}"/>
   </bookViews>
   <sheets>
     <sheet name="User Stories" sheetId="1" r:id="rId1"/>
     <sheet name="Mapping" sheetId="6" r:id="rId2"/>
-    <sheet name="Security Requirements" sheetId="2" r:id="rId3"/>
-    <sheet name="User Requirements" sheetId="3" r:id="rId4"/>
-    <sheet name="Planet Requirements" sheetId="4" r:id="rId5"/>
-    <sheet name="Moon Requirements" sheetId="5" r:id="rId6"/>
+    <sheet name="Acceptance Criteria" sheetId="7" r:id="rId3"/>
+    <sheet name="Security Requirements" sheetId="2" r:id="rId4"/>
+    <sheet name="User Requirements" sheetId="3" r:id="rId5"/>
+    <sheet name="Planet Requirements" sheetId="4" r:id="rId6"/>
+    <sheet name="Moon Requirements" sheetId="5" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="69">
   <si>
     <t>ID</t>
   </si>
@@ -224,14 +225,186 @@
   </si>
   <si>
     <t>To Be Continued!</t>
+  </si>
+  <si>
+    <t>Steps</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Given</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> the user is on the login page</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>When</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> the user clicks the register link</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>When</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> the user provides a valid username</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>And</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> the user provides a valid password</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>And</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> the user submits the credentials</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Then</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> the user should get a browser alert saying "Account created successfully"</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">And </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>the user should be redirected to the login page</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
@@ -264,8 +437,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -349,19 +522,25 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7A75172B-577E-4D84-AF49-87F5C4778595}" name="Table1" displayName="Table1" ref="A1:B6" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7A75172B-577E-4D84-AF49-87F5C4778595}" name="Table1" displayName="Table1" ref="A1:B6" totalsRowShown="0" headerRowDxfId="20" dataDxfId="19">
   <autoFilter ref="A1:B6" xr:uid="{7A75172B-577E-4D84-AF49-87F5C4778595}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{FED0608C-55BC-4321-8720-E641D878198E}" name="ID" dataDxfId="2"/>
-    <tableColumn id="2" xr3:uid="{5B7B44D4-81F7-4CA6-98CC-2C160723D4F2}" name="User Story" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{FED0608C-55BC-4321-8720-E641D878198E}" name="ID" dataDxfId="18"/>
+    <tableColumn id="2" xr3:uid="{5B7B44D4-81F7-4CA6-98CC-2C160723D4F2}" name="User Story" dataDxfId="17"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{8C7A2EF1-1E3B-497A-963A-1E4B297B1AD8}" name="Table6" displayName="Table6" ref="A1:B11" totalsRowShown="0" headerRowDxfId="0">
-  <autoFilter ref="A1:B11" xr:uid="{8C7A2EF1-1E3B-497A-963A-1E4B297B1AD8}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{8C7A2EF1-1E3B-497A-963A-1E4B297B1AD8}" name="Table6" displayName="Table6" ref="A1:B11" totalsRowShown="0" headerRowDxfId="16">
+  <autoFilter ref="A1:B11" xr:uid="{8C7A2EF1-1E3B-497A-963A-1E4B297B1AD8}">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="US1"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{3E1D6F9B-CF49-4C23-A4F1-14FC88593279}" name="User Story"/>
     <tableColumn id="2" xr3:uid="{0AE99736-D95C-4721-996D-FB61185AF45C}" name="Requirement"/>
@@ -371,44 +550,44 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{CF32EC7D-69C5-4A93-8A2D-DC6765B2E759}" name="Table2" displayName="Table2" ref="A1:B4" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{CF32EC7D-69C5-4A93-8A2D-DC6765B2E759}" name="Table2" displayName="Table2" ref="A1:B4" totalsRowShown="0" headerRowDxfId="15" dataDxfId="14">
   <autoFilter ref="A1:B4" xr:uid="{CF32EC7D-69C5-4A93-8A2D-DC6765B2E759}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{516DE414-3CB5-42C3-B197-5FD33F813523}" name="ID" dataDxfId="6"/>
-    <tableColumn id="2" xr3:uid="{6D770425-64E8-434C-8D03-6414A09F53EC}" name="Security Requirement" dataDxfId="5"/>
+    <tableColumn id="1" xr3:uid="{516DE414-3CB5-42C3-B197-5FD33F813523}" name="ID" dataDxfId="13"/>
+    <tableColumn id="2" xr3:uid="{6D770425-64E8-434C-8D03-6414A09F53EC}" name="Security Requirement" dataDxfId="12"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{402AD37E-496A-4B82-BD5A-DDA158D6DA5D}" name="Table3" displayName="Table3" ref="A1:B7" totalsRowShown="0" headerRowDxfId="17" dataDxfId="18">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{402AD37E-496A-4B82-BD5A-DDA158D6DA5D}" name="Table3" displayName="Table3" ref="A1:B7" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
   <autoFilter ref="A1:B7" xr:uid="{402AD37E-496A-4B82-BD5A-DDA158D6DA5D}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{77E4F913-7B38-4531-8FAA-D16B0FAAB464}" name="ID" dataDxfId="20"/>
-    <tableColumn id="2" xr3:uid="{85281BD9-33CE-4F6C-84B3-1E17141FF66A}" name="User Requirement" dataDxfId="19"/>
+    <tableColumn id="1" xr3:uid="{77E4F913-7B38-4531-8FAA-D16B0FAAB464}" name="ID" dataDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{85281BD9-33CE-4F6C-84B3-1E17141FF66A}" name="User Requirement" dataDxfId="8"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{79042BBB-0F12-4F67-90F0-C8062A2B8101}" name="Table4" displayName="Table4" ref="A1:B7" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{79042BBB-0F12-4F67-90F0-C8062A2B8101}" name="Table4" displayName="Table4" ref="A1:B7" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
   <autoFilter ref="A1:B7" xr:uid="{79042BBB-0F12-4F67-90F0-C8062A2B8101}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{EC350D5A-6EAD-426C-A18A-35EC1B171BC1}" name="ID" dataDxfId="16"/>
-    <tableColumn id="2" xr3:uid="{690F5785-7E7F-4D6A-8A10-FEEAAFDE3874}" name="Planet Requirement" dataDxfId="15"/>
+    <tableColumn id="1" xr3:uid="{EC350D5A-6EAD-426C-A18A-35EC1B171BC1}" name="ID" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{690F5785-7E7F-4D6A-8A10-FEEAAFDE3874}" name="Planet Requirement" dataDxfId="4"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{CB73B250-B846-4BAF-AF3B-5117DBBA4973}" name="Table5" displayName="Table5" ref="A1:B8" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{CB73B250-B846-4BAF-AF3B-5117DBBA4973}" name="Table5" displayName="Table5" ref="A1:B8" totalsRowShown="0" headerRowDxfId="3" dataDxfId="2">
   <autoFilter ref="A1:B8" xr:uid="{CB73B250-B846-4BAF-AF3B-5117DBBA4973}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{486EA324-F847-400D-80A5-266D5E36FC20}" name="ID" dataDxfId="12"/>
-    <tableColumn id="2" xr3:uid="{96D5BDBF-2AB3-4652-A2F0-CF69353F8D08}" name="Moon Requirement" dataDxfId="11"/>
+    <tableColumn id="1" xr3:uid="{486EA324-F847-400D-80A5-266D5E36FC20}" name="ID" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{96D5BDBF-2AB3-4652-A2F0-CF69353F8D08}" name="Moon Requirement" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -734,7 +913,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:B3"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -746,50 +925,50 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="1" t="s">
         <v>6</v>
       </c>
     </row>
@@ -805,8 +984,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{751CFA12-0342-4856-9D1B-B622A006DBE5}">
   <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -879,7 +1058,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -887,7 +1066,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -895,6 +1074,7 @@
         <v>18</v>
       </c>
     </row>
+    <row r="11" spans="1:2" hidden="1" x14ac:dyDescent="0.25"/>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>60</v>
@@ -909,6 +1089,71 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E14EEDEC-6C50-4FA1-BB35-C40D70D716CC}">
+  <dimension ref="A1:B8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="27.5703125" customWidth="1"/>
+    <col min="2" max="2" width="42" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B3" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B4" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B5" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B6" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="B7" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="B8" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4F326BC-F067-41E8-847E-757ABB716A4D}">
   <dimension ref="A1:B5"/>
   <sheetViews>
@@ -967,7 +1212,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34D5955B-CBB4-4821-99BF-DB0B1EC1B1EA}">
   <dimension ref="A1:B8"/>
   <sheetViews>
@@ -1049,7 +1294,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46FBBBD4-BA32-4762-983D-1911FDD83C85}">
   <dimension ref="A1:B9"/>
   <sheetViews>
@@ -1134,7 +1379,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A2FE8F8-EFC1-44EB-82E1-9A97A755E2C6}">
   <dimension ref="A1:B9"/>
   <sheetViews>

</xml_diff>

<commit_message>
adding acceptance criteria examples to rtm
</commit_message>
<xml_diff>
--- a/Project 1/Example RTM.xlsx
+++ b/Project 1/Example RTM.xlsx
@@ -8,18 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EricSuminski\Desktop\241209-JWA\Project 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D64639A-A73D-426D-A8FF-183510A411CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B42F9F7-621B-4256-92F4-9F6970E88F21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="2" xr2:uid="{F782749A-F44B-4770-ADC0-B107849E38C9}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="4" xr2:uid="{F782749A-F44B-4770-ADC0-B107849E38C9}"/>
   </bookViews>
   <sheets>
     <sheet name="User Stories" sheetId="1" r:id="rId1"/>
     <sheet name="Mapping" sheetId="6" r:id="rId2"/>
-    <sheet name="Acceptance Criteria" sheetId="7" r:id="rId3"/>
-    <sheet name="Security Requirements" sheetId="2" r:id="rId4"/>
-    <sheet name="User Requirements" sheetId="3" r:id="rId5"/>
-    <sheet name="Planet Requirements" sheetId="4" r:id="rId6"/>
-    <sheet name="Moon Requirements" sheetId="5" r:id="rId7"/>
+    <sheet name="Acceptance Criteria General" sheetId="9" r:id="rId3"/>
+    <sheet name="Acceptance Criteria Short" sheetId="7" r:id="rId4"/>
+    <sheet name="Acceptance Criteria Long" sheetId="8" r:id="rId5"/>
+    <sheet name="Security Requirements" sheetId="2" r:id="rId6"/>
+    <sheet name="User Requirements" sheetId="3" r:id="rId7"/>
+    <sheet name="Planet Requirements" sheetId="4" r:id="rId8"/>
+    <sheet name="Moon Requirements" sheetId="5" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -42,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="89">
   <si>
     <t>ID</t>
   </si>
@@ -389,6 +391,339 @@
       </rPr>
       <t>the user should be redirected to the login page</t>
     </r>
+  </si>
+  <si>
+    <t>Acceptance Type</t>
+  </si>
+  <si>
+    <t>Positive</t>
+  </si>
+  <si>
+    <t>Negative</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>When</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> the user provides valid credentials</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>When</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> the user provides invalid username</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Then</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> the user should get a browser alert saying "Invalid username"</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>And</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> the user should stay on the registration page</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>And</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> the user provides an invalid password</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Then</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> the user should get a browser alert saying "Invalid password"</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>When</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> the user provides an  invalid username</t>
+    </r>
+  </si>
+  <si>
+    <t>"&lt;&gt;" can be used to indicate placeholders in your acceptance criteria. This can be useful if you need to accommodate similar but different acceptance criteria steps and reduce the overall number of steps you write out</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>And</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> the user provides password </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"&lt;password&gt;"</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Then</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> the user should get a browser alert saying </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"&lt;alert&gt;"</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>When</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> the user provides username </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"&lt;username input&gt;"</t>
+    </r>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>Easy to associate code to acceptance criteria</t>
+  </si>
+  <si>
+    <t>Easy to associate code to acceptance criteria, but will involve writing out more code than the short option</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">When </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>the user provides one or more invalid credentials</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Then</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> the user should get a browser alert saying a credential is invalid</t>
+    </r>
+  </si>
+  <si>
+    <t>Requires a bit more work to associate acceptance criteria to code</t>
   </si>
 </sst>
 </file>
@@ -412,12 +747,24 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -432,13 +779,28 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1089,71 +1451,604 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E14EEDEC-6C50-4FA1-BB35-C40D70D716CC}">
-  <dimension ref="A1:B8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1DB7E24-71A0-45E8-B6FE-84B6B441D184}">
+  <dimension ref="A1:D15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.5703125" customWidth="1"/>
-    <col min="2" max="2" width="42" customWidth="1"/>
+    <col min="1" max="1" width="12.28515625" customWidth="1"/>
+    <col min="2" max="2" width="17.5703125" customWidth="1"/>
+    <col min="3" max="3" width="36.85546875" customWidth="1"/>
+    <col min="4" max="4" width="54.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="D1" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B3" s="2" t="s">
+      <c r="D2" s="5"/>
+    </row>
+    <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="4"/>
+      <c r="B3" s="6"/>
+      <c r="C3" s="1" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B4" s="2" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B5" s="2" t="s">
+      <c r="D3" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="4"/>
+      <c r="B4" s="6"/>
+      <c r="C4" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="4"/>
+      <c r="B5" s="6"/>
+      <c r="C5" s="1" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B6" s="2" t="s">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="4"/>
+      <c r="B6" s="6"/>
+      <c r="C6" s="1" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="B7" s="2" t="s">
+    <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="4"/>
+      <c r="B7" s="6"/>
+      <c r="C7" s="1" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="B8" s="2" t="s">
+    <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="4"/>
+      <c r="B8" s="6"/>
+      <c r="C8" s="1" t="s">
         <v>68</v>
       </c>
     </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="4"/>
+      <c r="B9" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="4"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="4"/>
+      <c r="B11" s="7"/>
+      <c r="C11" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="4"/>
+      <c r="B12" s="7"/>
+      <c r="C12" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="4"/>
+      <c r="B13" s="7"/>
+      <c r="C13" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="4"/>
+      <c r="B14" s="7"/>
+      <c r="C14" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="2"/>
+    </row>
   </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="B2:B8"/>
+    <mergeCell ref="B9:B14"/>
+    <mergeCell ref="A2:A14"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E14EEDEC-6C50-4FA1-BB35-C40D70D716CC}">
+  <dimension ref="A1:G29"/>
+  <sheetViews>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.28515625" customWidth="1"/>
+    <col min="2" max="2" width="17.5703125" customWidth="1"/>
+    <col min="3" max="3" width="36.85546875" customWidth="1"/>
+    <col min="4" max="4" width="54.85546875" customWidth="1"/>
+    <col min="5" max="5" width="45.85546875" customWidth="1"/>
+    <col min="7" max="7" width="22.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="E1" s="1"/>
+      <c r="G1" s="1"/>
+    </row>
+    <row r="2" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="E2" s="1"/>
+      <c r="G2" s="5"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="4"/>
+      <c r="B3" s="6"/>
+      <c r="C3" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="E3" s="1"/>
+    </row>
+    <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="4"/>
+      <c r="B4" s="6"/>
+      <c r="C4" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="E4" s="1"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="4"/>
+      <c r="B5" s="6"/>
+      <c r="C5" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="E5" s="1"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="4"/>
+      <c r="B6" s="6"/>
+      <c r="C6" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E6" s="1"/>
+    </row>
+    <row r="7" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="4"/>
+      <c r="B7" s="6"/>
+      <c r="C7" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E7" s="1"/>
+    </row>
+    <row r="8" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="4"/>
+      <c r="B8" s="6"/>
+      <c r="C8" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="E8" s="1"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="4"/>
+      <c r="B9" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="4"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="4"/>
+      <c r="B11" s="7"/>
+      <c r="C11" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="E11" s="1"/>
+    </row>
+    <row r="12" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="4"/>
+      <c r="B12" s="7"/>
+      <c r="C12" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="E12" s="1"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="4"/>
+      <c r="B13" s="7"/>
+      <c r="C13" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E13" s="1"/>
+    </row>
+    <row r="14" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="4"/>
+      <c r="B14" s="7"/>
+      <c r="C14" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="E14" s="1"/>
+    </row>
+    <row r="15" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="4"/>
+      <c r="B15" s="7"/>
+      <c r="C15" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E15" s="1"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="2"/>
+      <c r="C16" s="1"/>
+      <c r="E16" s="1"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="2"/>
+      <c r="C17" s="1"/>
+      <c r="E17" s="1"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="2"/>
+      <c r="C18" s="1"/>
+      <c r="E18" s="1"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="2"/>
+      <c r="C19" s="1"/>
+      <c r="E19" s="1"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="2"/>
+      <c r="C20" s="1"/>
+      <c r="E20" s="1"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="2"/>
+      <c r="C21" s="1"/>
+      <c r="E21" s="1"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="2"/>
+      <c r="C22" s="1"/>
+      <c r="E22" s="1"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="2"/>
+      <c r="C23" s="1"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="2"/>
+      <c r="C24" s="1"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="2"/>
+      <c r="C25" s="1"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="2"/>
+      <c r="C26" s="1"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="2"/>
+      <c r="C27" s="1"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="2"/>
+      <c r="C28" s="1"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="2"/>
+      <c r="C29" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A2:A15"/>
+    <mergeCell ref="B2:B8"/>
+    <mergeCell ref="B9:B15"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9F5FABA-1ABC-4F95-8F7C-37C42F38162D}">
+  <dimension ref="A1:D29"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.5703125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="18.85546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="36.85546875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="45.7109375" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B3" s="6"/>
+      <c r="C3" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="B4" s="6"/>
+      <c r="C4" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B5" s="6"/>
+      <c r="C5" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B6" s="6"/>
+      <c r="C6" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="B7" s="6"/>
+      <c r="C7" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="B8" s="6"/>
+      <c r="C8" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B9" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B10" s="7"/>
+      <c r="C10" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="B11" s="7"/>
+      <c r="C11" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B12" s="7"/>
+      <c r="C12" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B13" s="7"/>
+      <c r="C13" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="B14" s="7"/>
+      <c r="C14" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="B15" s="7"/>
+      <c r="C15" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B16" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B17" s="7"/>
+      <c r="C17" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="B18" s="7"/>
+      <c r="C18" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="B19" s="7"/>
+      <c r="C19" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B20" s="7"/>
+      <c r="C20" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="B21" s="7"/>
+      <c r="C21" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="B22" s="7"/>
+      <c r="C22" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B23" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B24" s="7"/>
+      <c r="C24" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="25" spans="2:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="B25" s="7"/>
+      <c r="C25" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="26" spans="2:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="B26" s="7"/>
+      <c r="C26" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B27" s="7"/>
+      <c r="C27" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="28" spans="2:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="B28" s="7"/>
+      <c r="C28" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="29" spans="2:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="B29" s="7"/>
+      <c r="C29" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="B2:B8"/>
+    <mergeCell ref="B9:B15"/>
+    <mergeCell ref="B16:B22"/>
+    <mergeCell ref="B23:B29"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4F326BC-F067-41E8-847E-757ABB716A4D}">
   <dimension ref="A1:B5"/>
   <sheetViews>
@@ -1212,7 +2107,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34D5955B-CBB4-4821-99BF-DB0B1EC1B1EA}">
   <dimension ref="A1:B8"/>
   <sheetViews>
@@ -1294,7 +2189,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46FBBBD4-BA32-4762-983D-1911FDD83C85}">
   <dimension ref="A1:B9"/>
   <sheetViews>
@@ -1379,7 +2274,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A2FE8F8-EFC1-44EB-82E1-9A97A755E2C6}">
   <dimension ref="A1:B9"/>
   <sheetViews>

</xml_diff>

<commit_message>
updating example rtm with more content
</commit_message>
<xml_diff>
--- a/Project 1/Example RTM.xlsx
+++ b/Project 1/Example RTM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EricSuminski\Desktop\241209-JWA\Project 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B42F9F7-621B-4256-92F4-9F6970E88F21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{320F32A6-14B8-43C0-AB42-57D463DB0369}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="4" xr2:uid="{F782749A-F44B-4770-ADC0-B107849E38C9}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="2" xr2:uid="{F782749A-F44B-4770-ADC0-B107849E38C9}"/>
   </bookViews>
   <sheets>
     <sheet name="User Stories" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="95">
   <si>
     <t>ID</t>
   </si>
@@ -724,6 +724,124 @@
   </si>
   <si>
     <t>Requires a bit more work to associate acceptance criteria to code</t>
+  </si>
+  <si>
+    <t>negative</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>When</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> the user logs in</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Then</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> they should see their planets and moons</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Given</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> the user is not logged in</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>When</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> the user tries to directly access the home page</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Then</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> the user should be denied access</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -779,7 +897,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -791,9 +909,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -801,6 +916,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -895,8 +1019,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{8C7A2EF1-1E3B-497A-963A-1E4B297B1AD8}" name="Table6" displayName="Table6" ref="A1:B11" totalsRowShown="0" headerRowDxfId="16">
-  <autoFilter ref="A1:B11" xr:uid="{8C7A2EF1-1E3B-497A-963A-1E4B297B1AD8}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{8C7A2EF1-1E3B-497A-963A-1E4B297B1AD8}" name="Table6" displayName="Table6" ref="A1:B15" totalsRowShown="0" headerRowDxfId="16">
+  <autoFilter ref="A1:B15" xr:uid="{8C7A2EF1-1E3B-497A-963A-1E4B297B1AD8}">
     <filterColumn colId="0">
       <filters>
         <filter val="US1"/>
@@ -1344,10 +1468,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{751CFA12-0342-4856-9D1B-B622A006DBE5}">
-  <dimension ref="A1:B13"/>
+  <dimension ref="A1:B22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B8"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1437,8 +1561,40 @@
       </c>
     </row>
     <row r="11" spans="1:2" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12" t="s">
+        <v>17</v>
+      </c>
+    </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B13" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>9</v>
+      </c>
+      <c r="B14" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>9</v>
+      </c>
+      <c r="B15" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>60</v>
       </c>
     </row>
@@ -1452,10 +1608,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1DB7E24-71A0-45E8-B6FE-84B6B441D184}">
-  <dimension ref="A1:D15"/>
+  <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1481,20 +1637,20 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="5" t="s">
         <v>70</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="D2" s="5"/>
+      <c r="D2" s="4"/>
     </row>
     <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="4"/>
-      <c r="B3" s="6"/>
+      <c r="A3" s="7"/>
+      <c r="B3" s="5"/>
       <c r="C3" s="1" t="s">
         <v>63</v>
       </c>
@@ -1503,43 +1659,43 @@
       </c>
     </row>
     <row r="4" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="4"/>
-      <c r="B4" s="6"/>
+      <c r="A4" s="7"/>
+      <c r="B4" s="5"/>
       <c r="C4" s="1" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="4"/>
-      <c r="B5" s="6"/>
+      <c r="A5" s="7"/>
+      <c r="B5" s="5"/>
       <c r="C5" s="1" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="4"/>
-      <c r="B6" s="6"/>
+      <c r="A6" s="7"/>
+      <c r="B6" s="5"/>
       <c r="C6" s="1" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="4"/>
-      <c r="B7" s="6"/>
+      <c r="A7" s="7"/>
+      <c r="B7" s="5"/>
       <c r="C7" s="1" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="4"/>
-      <c r="B8" s="6"/>
+      <c r="A8" s="7"/>
+      <c r="B8" s="5"/>
       <c r="C8" s="1" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="4"/>
-      <c r="B9" s="7" t="s">
+      <c r="A9" s="7"/>
+      <c r="B9" s="6" t="s">
         <v>71</v>
       </c>
       <c r="C9" s="1" t="s">
@@ -1547,48 +1703,96 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="4"/>
-      <c r="B10" s="7"/>
+      <c r="A10" s="7"/>
+      <c r="B10" s="6"/>
       <c r="C10" s="1" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="4"/>
-      <c r="B11" s="7"/>
+      <c r="A11" s="7"/>
+      <c r="B11" s="6"/>
       <c r="C11" s="1" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="4"/>
-      <c r="B12" s="7"/>
+      <c r="A12" s="7"/>
+      <c r="B12" s="6"/>
       <c r="C12" s="1" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="4"/>
-      <c r="B13" s="7"/>
+      <c r="A13" s="7"/>
+      <c r="B13" s="6"/>
       <c r="C13" s="1" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="4"/>
-      <c r="B14" s="7"/>
+      <c r="A14" s="7"/>
+      <c r="B14" s="6"/>
       <c r="C14" s="1" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="2"/>
+      <c r="A15" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="7"/>
+      <c r="B16" s="8"/>
+      <c r="C16" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="7"/>
+      <c r="B17" s="8"/>
+      <c r="C17" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="7"/>
+      <c r="B18" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="7"/>
+      <c r="B19" s="9"/>
+      <c r="C19" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="7"/>
+      <c r="B20" s="9"/>
+      <c r="C20" s="1" t="s">
+        <v>94</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="6">
     <mergeCell ref="B2:B8"/>
     <mergeCell ref="B9:B14"/>
     <mergeCell ref="A2:A14"/>
+    <mergeCell ref="A15:A20"/>
+    <mergeCell ref="B15:B17"/>
+    <mergeCell ref="B18:B20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1629,24 +1833,24 @@
       <c r="G1" s="1"/>
     </row>
     <row r="2" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="5" t="s">
         <v>70</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="4" t="s">
         <v>79</v>
       </c>
       <c r="E2" s="1"/>
-      <c r="G2" s="5"/>
+      <c r="G2" s="4"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="4"/>
-      <c r="B3" s="6"/>
+      <c r="A3" s="7"/>
+      <c r="B3" s="5"/>
       <c r="C3" s="1" t="s">
         <v>63</v>
       </c>
@@ -1656,48 +1860,48 @@
       <c r="E3" s="1"/>
     </row>
     <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="4"/>
-      <c r="B4" s="6"/>
+      <c r="A4" s="7"/>
+      <c r="B4" s="5"/>
       <c r="C4" s="1" t="s">
         <v>72</v>
       </c>
       <c r="E4" s="1"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="4"/>
-      <c r="B5" s="6"/>
+      <c r="A5" s="7"/>
+      <c r="B5" s="5"/>
       <c r="C5" s="1" t="s">
         <v>65</v>
       </c>
       <c r="E5" s="1"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="4"/>
-      <c r="B6" s="6"/>
+      <c r="A6" s="7"/>
+      <c r="B6" s="5"/>
       <c r="C6" s="1" t="s">
         <v>66</v>
       </c>
       <c r="E6" s="1"/>
     </row>
     <row r="7" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="4"/>
-      <c r="B7" s="6"/>
+      <c r="A7" s="7"/>
+      <c r="B7" s="5"/>
       <c r="C7" s="1" t="s">
         <v>67</v>
       </c>
       <c r="E7" s="1"/>
     </row>
     <row r="8" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="4"/>
-      <c r="B8" s="6"/>
+      <c r="A8" s="7"/>
+      <c r="B8" s="5"/>
       <c r="C8" s="1" t="s">
         <v>68</v>
       </c>
       <c r="E8" s="1"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="4"/>
-      <c r="B9" s="7" t="s">
+      <c r="A9" s="7"/>
+      <c r="B9" s="6" t="s">
         <v>71</v>
       </c>
       <c r="C9" s="1" t="s">
@@ -1705,47 +1909,47 @@
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="4"/>
-      <c r="B10" s="7"/>
+      <c r="A10" s="7"/>
+      <c r="B10" s="6"/>
       <c r="C10" s="1" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="4"/>
-      <c r="B11" s="7"/>
+      <c r="A11" s="7"/>
+      <c r="B11" s="6"/>
       <c r="C11" s="1" t="s">
         <v>82</v>
       </c>
       <c r="E11" s="1"/>
     </row>
     <row r="12" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="4"/>
-      <c r="B12" s="7"/>
+      <c r="A12" s="7"/>
+      <c r="B12" s="6"/>
       <c r="C12" s="1" t="s">
         <v>80</v>
       </c>
       <c r="E12" s="1"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="4"/>
-      <c r="B13" s="7"/>
+      <c r="A13" s="7"/>
+      <c r="B13" s="6"/>
       <c r="C13" s="1" t="s">
         <v>66</v>
       </c>
       <c r="E13" s="1"/>
     </row>
     <row r="14" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="4"/>
-      <c r="B14" s="7"/>
+      <c r="A14" s="7"/>
+      <c r="B14" s="6"/>
       <c r="C14" s="1" t="s">
         <v>81</v>
       </c>
       <c r="E14" s="1"/>
     </row>
     <row r="15" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="4"/>
-      <c r="B15" s="7"/>
+      <c r="A15" s="7"/>
+      <c r="B15" s="6"/>
       <c r="C15" s="1" t="s">
         <v>75</v>
       </c>
@@ -1828,7 +2032,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9F5FABA-1ABC-4F95-8F7C-37C42F38162D}">
   <dimension ref="A1:D29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
@@ -1859,7 +2063,7 @@
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="5" t="s">
         <v>70</v>
       </c>
       <c r="C2" s="1" t="s">
@@ -1870,43 +2074,43 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B3" s="6"/>
+      <c r="B3" s="5"/>
       <c r="C3" s="1" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="B4" s="6"/>
+      <c r="B4" s="5"/>
       <c r="C4" s="1" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B5" s="6"/>
+      <c r="B5" s="5"/>
       <c r="C5" s="1" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B6" s="6"/>
+      <c r="B6" s="5"/>
       <c r="C6" s="1" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="B7" s="6"/>
+      <c r="B7" s="5"/>
       <c r="C7" s="1" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="B8" s="6"/>
+      <c r="B8" s="5"/>
       <c r="C8" s="1" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B9" s="7" t="s">
+      <c r="B9" s="6" t="s">
         <v>71</v>
       </c>
       <c r="C9" s="1" t="s">
@@ -1914,43 +2118,43 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B10" s="7"/>
+      <c r="B10" s="6"/>
       <c r="C10" s="1" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="B11" s="7"/>
+      <c r="B11" s="6"/>
       <c r="C11" s="1" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B12" s="7"/>
+      <c r="B12" s="6"/>
       <c r="C12" s="1" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B13" s="7"/>
+      <c r="B13" s="6"/>
       <c r="C13" s="1" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="B14" s="7"/>
+      <c r="B14" s="6"/>
       <c r="C14" s="1" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="B15" s="7"/>
+      <c r="B15" s="6"/>
       <c r="C15" s="1" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B16" s="7" t="s">
+      <c r="B16" s="6" t="s">
         <v>71</v>
       </c>
       <c r="C16" s="1" t="s">
@@ -1958,43 +2162,43 @@
       </c>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B17" s="7"/>
+      <c r="B17" s="6"/>
       <c r="C17" s="1" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="18" spans="2:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="B18" s="7"/>
+      <c r="B18" s="6"/>
       <c r="C18" s="1" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="19" spans="2:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="B19" s="7"/>
+      <c r="B19" s="6"/>
       <c r="C19" s="1" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B20" s="7"/>
+      <c r="B20" s="6"/>
       <c r="C20" s="1" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="21" spans="2:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="B21" s="7"/>
+      <c r="B21" s="6"/>
       <c r="C21" s="1" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="22" spans="2:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="B22" s="7"/>
+      <c r="B22" s="6"/>
       <c r="C22" s="1" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="23" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B23" s="7" t="s">
+      <c r="B23" s="6" t="s">
         <v>71</v>
       </c>
       <c r="C23" s="1" t="s">
@@ -2002,37 +2206,37 @@
       </c>
     </row>
     <row r="24" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B24" s="7"/>
+      <c r="B24" s="6"/>
       <c r="C24" s="1" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="25" spans="2:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="B25" s="7"/>
+      <c r="B25" s="6"/>
       <c r="C25" s="1" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="26" spans="2:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="B26" s="7"/>
+      <c r="B26" s="6"/>
       <c r="C26" s="1" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="27" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B27" s="7"/>
+      <c r="B27" s="6"/>
       <c r="C27" s="1" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="28" spans="2:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="B28" s="7"/>
+      <c r="B28" s="6"/>
       <c r="C28" s="1" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="29" spans="2:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="B29" s="7"/>
+      <c r="B29" s="6"/>
       <c r="C29" s="1" t="s">
         <v>75</v>
       </c>
@@ -2053,7 +2257,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:B4"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2194,7 +2398,7 @@
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2278,7 +2482,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A2FE8F8-EFC1-44EB-82E1-9A97A755E2C6}">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A3" workbookViewId="0">
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
adding test case design notes and resources
</commit_message>
<xml_diff>
--- a/Project 1/Example RTM.xlsx
+++ b/Project 1/Example RTM.xlsx
@@ -8,20 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EricSuminski\Desktop\241209-JWA\Project 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{320F32A6-14B8-43C0-AB42-57D463DB0369}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4979595C-5287-4F66-A59F-8E4A155AB351}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="2" xr2:uid="{F782749A-F44B-4770-ADC0-B107849E38C9}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" firstSheet="3" activeTab="5" xr2:uid="{F782749A-F44B-4770-ADC0-B107849E38C9}"/>
   </bookViews>
   <sheets>
     <sheet name="User Stories" sheetId="1" r:id="rId1"/>
     <sheet name="Mapping" sheetId="6" r:id="rId2"/>
-    <sheet name="Acceptance Criteria General" sheetId="9" r:id="rId3"/>
-    <sheet name="Acceptance Criteria Short" sheetId="7" r:id="rId4"/>
-    <sheet name="Acceptance Criteria Long" sheetId="8" r:id="rId5"/>
-    <sheet name="Security Requirements" sheetId="2" r:id="rId6"/>
-    <sheet name="User Requirements" sheetId="3" r:id="rId7"/>
-    <sheet name="Planet Requirements" sheetId="4" r:id="rId8"/>
-    <sheet name="Moon Requirements" sheetId="5" r:id="rId9"/>
+    <sheet name="Test Data" sheetId="10" r:id="rId3"/>
+    <sheet name="Acceptance Criteria General" sheetId="9" r:id="rId4"/>
+    <sheet name="Acceptance Criteria Short" sheetId="7" r:id="rId5"/>
+    <sheet name="Acceptance Criteria Long" sheetId="8" r:id="rId6"/>
+    <sheet name="Security Requirements" sheetId="2" r:id="rId7"/>
+    <sheet name="User Requirements" sheetId="3" r:id="rId8"/>
+    <sheet name="Planet Requirements" sheetId="4" r:id="rId9"/>
+    <sheet name="Moon Requirements" sheetId="5" r:id="rId10"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -44,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="95">
   <si>
     <t>ID</t>
   </si>
@@ -1466,12 +1467,102 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A2FE8F8-EFC1-44EB-82E1-9A97A755E2C6}">
+  <dimension ref="A1:B9"/>
+  <sheetViews>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="27.28515625" customWidth="1"/>
+    <col min="2" max="2" width="27.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{751CFA12-0342-4856-9D1B-B622A006DBE5}">
   <dimension ref="A1:B22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1560,39 +1651,39 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:2" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>9</v>
       </c>
       <c r="B12" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>9</v>
       </c>
       <c r="B13" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>9</v>
       </c>
       <c r="B14" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>9</v>
-      </c>
-      <c r="B15" t="s">
         <v>55</v>
       </c>
     </row>
+    <row r="15" spans="1:2" hidden="1" x14ac:dyDescent="0.25"/>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>60</v>
@@ -1607,11 +1698,28 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D4693EB-185E-4567-AC0C-8312035BA2A5}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="27.42578125" customWidth="1"/>
+    <col min="2" max="2" width="27.5703125" customWidth="1"/>
+    <col min="3" max="3" width="28" customWidth="1"/>
+  </cols>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1DB7E24-71A0-45E8-B6FE-84B6B441D184}">
   <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1669,29 +1777,25 @@
       <c r="A5" s="7"/>
       <c r="B5" s="5"/>
       <c r="C5" s="1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="7"/>
       <c r="B6" s="5"/>
       <c r="C6" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="7"/>
       <c r="B7" s="5"/>
       <c r="C7" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="7"/>
-      <c r="B8" s="5"/>
-      <c r="C8" s="1" t="s">
-        <v>68</v>
-      </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="7"/>
@@ -1787,23 +1891,23 @@
     </row>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="B2:B8"/>
     <mergeCell ref="B9:B14"/>
     <mergeCell ref="A2:A14"/>
     <mergeCell ref="A15:A20"/>
     <mergeCell ref="B15:B17"/>
     <mergeCell ref="B18:B20"/>
+    <mergeCell ref="B2:B7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E14EEDEC-6C50-4FA1-BB35-C40D70D716CC}">
   <dimension ref="A1:G29"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1863,7 +1967,7 @@
       <c r="A4" s="7"/>
       <c r="B4" s="5"/>
       <c r="C4" s="1" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="E4" s="1"/>
     </row>
@@ -2028,12 +2132,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9F5FABA-1ABC-4F95-8F7C-37C42F38162D}">
   <dimension ref="A1:D29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2082,7 +2186,7 @@
     <row r="4" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B4" s="5"/>
       <c r="C4" s="1" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -2252,7 +2356,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4F326BC-F067-41E8-847E-757ABB716A4D}">
   <dimension ref="A1:B5"/>
   <sheetViews>
@@ -2311,12 +2415,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34D5955B-CBB4-4821-99BF-DB0B1EC1B1EA}">
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B7"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B4" sqref="B3:B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2393,7 +2497,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46FBBBD4-BA32-4762-983D-1911FDD83C85}">
   <dimension ref="A1:B9"/>
   <sheetViews>
@@ -2476,94 +2580,4 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A2FE8F8-EFC1-44EB-82E1-9A97A755E2C6}">
-  <dimension ref="A1:B9"/>
-  <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="27.28515625" customWidth="1"/>
-    <col min="2" max="2" width="27.42578125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
adding example of test data organization
</commit_message>
<xml_diff>
--- a/Project 1/Example RTM.xlsx
+++ b/Project 1/Example RTM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EricSuminski\Desktop\241209-JWA\Project 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4979595C-5287-4F66-A59F-8E4A155AB351}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFED0890-8954-4C3B-8BAD-15EA234DA922}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" firstSheet="3" activeTab="5" xr2:uid="{F782749A-F44B-4770-ADC0-B107849E38C9}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" firstSheet="5" activeTab="7" xr2:uid="{F782749A-F44B-4770-ADC0-B107849E38C9}"/>
   </bookViews>
   <sheets>
     <sheet name="User Stories" sheetId="1" r:id="rId1"/>
@@ -912,9 +912,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -926,6 +923,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1745,10 +1745,10 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="9" t="s">
         <v>70</v>
       </c>
       <c r="C2" s="1" t="s">
@@ -1757,8 +1757,8 @@
       <c r="D2" s="4"/>
     </row>
     <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="7"/>
-      <c r="B3" s="5"/>
+      <c r="A3" s="6"/>
+      <c r="B3" s="9"/>
       <c r="C3" s="1" t="s">
         <v>63</v>
       </c>
@@ -1767,39 +1767,39 @@
       </c>
     </row>
     <row r="4" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="7"/>
-      <c r="B4" s="5"/>
+      <c r="A4" s="6"/>
+      <c r="B4" s="9"/>
       <c r="C4" s="1" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="7"/>
-      <c r="B5" s="5"/>
+      <c r="A5" s="6"/>
+      <c r="B5" s="9"/>
       <c r="C5" s="1" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="7"/>
-      <c r="B6" s="5"/>
+      <c r="A6" s="6"/>
+      <c r="B6" s="9"/>
       <c r="C6" s="1" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="7"/>
-      <c r="B7" s="5"/>
+      <c r="A7" s="6"/>
+      <c r="B7" s="9"/>
       <c r="C7" s="1" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="7"/>
+      <c r="A8" s="6"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="7"/>
-      <c r="B9" s="6" t="s">
+      <c r="A9" s="6"/>
+      <c r="B9" s="5" t="s">
         <v>71</v>
       </c>
       <c r="C9" s="1" t="s">
@@ -1807,45 +1807,45 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="7"/>
-      <c r="B10" s="6"/>
+      <c r="A10" s="6"/>
+      <c r="B10" s="5"/>
       <c r="C10" s="1" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="7"/>
-      <c r="B11" s="6"/>
+      <c r="A11" s="6"/>
+      <c r="B11" s="5"/>
       <c r="C11" s="1" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="7"/>
-      <c r="B12" s="6"/>
+      <c r="A12" s="6"/>
+      <c r="B12" s="5"/>
       <c r="C12" s="1" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="7"/>
-      <c r="B13" s="6"/>
+      <c r="A13" s="6"/>
+      <c r="B13" s="5"/>
       <c r="C13" s="1" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="7"/>
-      <c r="B14" s="6"/>
+      <c r="A14" s="6"/>
+      <c r="B14" s="5"/>
       <c r="C14" s="1" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="7" t="s">
+      <c r="A15" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B15" s="8" t="s">
+      <c r="B15" s="7" t="s">
         <v>70</v>
       </c>
       <c r="C15" s="1" t="s">
@@ -1853,22 +1853,22 @@
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="7"/>
-      <c r="B16" s="8"/>
+      <c r="A16" s="6"/>
+      <c r="B16" s="7"/>
       <c r="C16" s="1" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="7"/>
-      <c r="B17" s="8"/>
+      <c r="A17" s="6"/>
+      <c r="B17" s="7"/>
       <c r="C17" s="1" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="7"/>
-      <c r="B18" s="9" t="s">
+      <c r="A18" s="6"/>
+      <c r="B18" s="8" t="s">
         <v>89</v>
       </c>
       <c r="C18" s="1" t="s">
@@ -1876,15 +1876,15 @@
       </c>
     </row>
     <row r="19" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A19" s="7"/>
-      <c r="B19" s="9"/>
+      <c r="A19" s="6"/>
+      <c r="B19" s="8"/>
       <c r="C19" s="1" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="7"/>
-      <c r="B20" s="9"/>
+      <c r="A20" s="6"/>
+      <c r="B20" s="8"/>
       <c r="C20" s="1" t="s">
         <v>94</v>
       </c>
@@ -1937,10 +1937,10 @@
       <c r="G1" s="1"/>
     </row>
     <row r="2" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="9" t="s">
         <v>70</v>
       </c>
       <c r="C2" s="1" t="s">
@@ -1953,8 +1953,8 @@
       <c r="G2" s="4"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="7"/>
-      <c r="B3" s="5"/>
+      <c r="A3" s="6"/>
+      <c r="B3" s="9"/>
       <c r="C3" s="1" t="s">
         <v>63</v>
       </c>
@@ -1964,48 +1964,48 @@
       <c r="E3" s="1"/>
     </row>
     <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="7"/>
-      <c r="B4" s="5"/>
+      <c r="A4" s="6"/>
+      <c r="B4" s="9"/>
       <c r="C4" s="1" t="s">
         <v>64</v>
       </c>
       <c r="E4" s="1"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="7"/>
-      <c r="B5" s="5"/>
+      <c r="A5" s="6"/>
+      <c r="B5" s="9"/>
       <c r="C5" s="1" t="s">
         <v>65</v>
       </c>
       <c r="E5" s="1"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="7"/>
-      <c r="B6" s="5"/>
+      <c r="A6" s="6"/>
+      <c r="B6" s="9"/>
       <c r="C6" s="1" t="s">
         <v>66</v>
       </c>
       <c r="E6" s="1"/>
     </row>
     <row r="7" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="7"/>
-      <c r="B7" s="5"/>
+      <c r="A7" s="6"/>
+      <c r="B7" s="9"/>
       <c r="C7" s="1" t="s">
         <v>67</v>
       </c>
       <c r="E7" s="1"/>
     </row>
     <row r="8" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="7"/>
-      <c r="B8" s="5"/>
+      <c r="A8" s="6"/>
+      <c r="B8" s="9"/>
       <c r="C8" s="1" t="s">
         <v>68</v>
       </c>
       <c r="E8" s="1"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="7"/>
-      <c r="B9" s="6" t="s">
+      <c r="A9" s="6"/>
+      <c r="B9" s="5" t="s">
         <v>71</v>
       </c>
       <c r="C9" s="1" t="s">
@@ -2013,47 +2013,47 @@
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="7"/>
-      <c r="B10" s="6"/>
+      <c r="A10" s="6"/>
+      <c r="B10" s="5"/>
       <c r="C10" s="1" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="7"/>
-      <c r="B11" s="6"/>
+      <c r="A11" s="6"/>
+      <c r="B11" s="5"/>
       <c r="C11" s="1" t="s">
         <v>82</v>
       </c>
       <c r="E11" s="1"/>
     </row>
     <row r="12" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="7"/>
-      <c r="B12" s="6"/>
+      <c r="A12" s="6"/>
+      <c r="B12" s="5"/>
       <c r="C12" s="1" t="s">
         <v>80</v>
       </c>
       <c r="E12" s="1"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="7"/>
-      <c r="B13" s="6"/>
+      <c r="A13" s="6"/>
+      <c r="B13" s="5"/>
       <c r="C13" s="1" t="s">
         <v>66</v>
       </c>
       <c r="E13" s="1"/>
     </row>
     <row r="14" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="7"/>
-      <c r="B14" s="6"/>
+      <c r="A14" s="6"/>
+      <c r="B14" s="5"/>
       <c r="C14" s="1" t="s">
         <v>81</v>
       </c>
       <c r="E14" s="1"/>
     </row>
     <row r="15" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="7"/>
-      <c r="B15" s="6"/>
+      <c r="A15" s="6"/>
+      <c r="B15" s="5"/>
       <c r="C15" s="1" t="s">
         <v>75</v>
       </c>
@@ -2136,7 +2136,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9F5FABA-1ABC-4F95-8F7C-37C42F38162D}">
   <dimension ref="A1:D29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
@@ -2167,7 +2167,7 @@
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="9" t="s">
         <v>70</v>
       </c>
       <c r="C2" s="1" t="s">
@@ -2178,43 +2178,43 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B3" s="5"/>
+      <c r="B3" s="9"/>
       <c r="C3" s="1" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="B4" s="5"/>
+      <c r="B4" s="9"/>
       <c r="C4" s="1" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B5" s="5"/>
+      <c r="B5" s="9"/>
       <c r="C5" s="1" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B6" s="5"/>
+      <c r="B6" s="9"/>
       <c r="C6" s="1" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="B7" s="5"/>
+      <c r="B7" s="9"/>
       <c r="C7" s="1" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="B8" s="5"/>
+      <c r="B8" s="9"/>
       <c r="C8" s="1" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="5" t="s">
         <v>71</v>
       </c>
       <c r="C9" s="1" t="s">
@@ -2222,43 +2222,43 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B10" s="6"/>
+      <c r="B10" s="5"/>
       <c r="C10" s="1" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="B11" s="6"/>
+      <c r="B11" s="5"/>
       <c r="C11" s="1" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B12" s="6"/>
+      <c r="B12" s="5"/>
       <c r="C12" s="1" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B13" s="6"/>
+      <c r="B13" s="5"/>
       <c r="C13" s="1" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="B14" s="6"/>
+      <c r="B14" s="5"/>
       <c r="C14" s="1" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="B15" s="6"/>
+      <c r="B15" s="5"/>
       <c r="C15" s="1" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B16" s="6" t="s">
+      <c r="B16" s="5" t="s">
         <v>71</v>
       </c>
       <c r="C16" s="1" t="s">
@@ -2266,43 +2266,43 @@
       </c>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B17" s="6"/>
+      <c r="B17" s="5"/>
       <c r="C17" s="1" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="18" spans="2:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="B18" s="6"/>
+      <c r="B18" s="5"/>
       <c r="C18" s="1" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="19" spans="2:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="B19" s="6"/>
+      <c r="B19" s="5"/>
       <c r="C19" s="1" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B20" s="6"/>
+      <c r="B20" s="5"/>
       <c r="C20" s="1" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="21" spans="2:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="B21" s="6"/>
+      <c r="B21" s="5"/>
       <c r="C21" s="1" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="22" spans="2:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="B22" s="6"/>
+      <c r="B22" s="5"/>
       <c r="C22" s="1" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="23" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B23" s="6" t="s">
+      <c r="B23" s="5" t="s">
         <v>71</v>
       </c>
       <c r="C23" s="1" t="s">
@@ -2310,37 +2310,37 @@
       </c>
     </row>
     <row r="24" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B24" s="6"/>
+      <c r="B24" s="5"/>
       <c r="C24" s="1" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="25" spans="2:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="B25" s="6"/>
+      <c r="B25" s="5"/>
       <c r="C25" s="1" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="26" spans="2:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="B26" s="6"/>
+      <c r="B26" s="5"/>
       <c r="C26" s="1" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="27" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B27" s="6"/>
+      <c r="B27" s="5"/>
       <c r="C27" s="1" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="28" spans="2:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="B28" s="6"/>
+      <c r="B28" s="5"/>
       <c r="C28" s="1" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="29" spans="2:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="B29" s="6"/>
+      <c r="B29" s="5"/>
       <c r="C29" s="1" t="s">
         <v>75</v>
       </c>
@@ -2419,8 +2419,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34D5955B-CBB4-4821-99BF-DB0B1EC1B1EA}">
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B4" sqref="B3:B4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6:B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
updating rtm with test data and decision tables for scenarios
</commit_message>
<xml_diff>
--- a/Project 1/Example RTM.xlsx
+++ b/Project 1/Example RTM.xlsx
@@ -8,21 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EricSuminski\Desktop\241209-JWA\Project 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFED0890-8954-4C3B-8BAD-15EA234DA922}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09D621E2-9468-4218-AC26-C2593D892B32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" firstSheet="5" activeTab="7" xr2:uid="{F782749A-F44B-4770-ADC0-B107849E38C9}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="4" xr2:uid="{F782749A-F44B-4770-ADC0-B107849E38C9}"/>
   </bookViews>
   <sheets>
     <sheet name="User Stories" sheetId="1" r:id="rId1"/>
-    <sheet name="Mapping" sheetId="6" r:id="rId2"/>
-    <sheet name="Test Data" sheetId="10" r:id="rId3"/>
+    <sheet name="Requirements" sheetId="11" r:id="rId2"/>
+    <sheet name="Mapping" sheetId="6" r:id="rId3"/>
     <sheet name="Acceptance Criteria General" sheetId="9" r:id="rId4"/>
-    <sheet name="Acceptance Criteria Short" sheetId="7" r:id="rId5"/>
-    <sheet name="Acceptance Criteria Long" sheetId="8" r:id="rId6"/>
-    <sheet name="Security Requirements" sheetId="2" r:id="rId7"/>
-    <sheet name="User Requirements" sheetId="3" r:id="rId8"/>
-    <sheet name="Planet Requirements" sheetId="4" r:id="rId9"/>
-    <sheet name="Moon Requirements" sheetId="5" r:id="rId10"/>
+    <sheet name="Test Data" sheetId="10" r:id="rId5"/>
+    <sheet name="Acceptance Criteria Short" sheetId="7" r:id="rId6"/>
+    <sheet name="Acceptance Criteria Long" sheetId="8" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -45,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="148">
   <si>
     <t>ID</t>
   </si>
@@ -843,13 +840,172 @@
       </rPr>
       <t xml:space="preserve"> the user should be denied access</t>
     </r>
+  </si>
+  <si>
+    <t>Positive Test Data</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>valid username</t>
+  </si>
+  <si>
+    <t>VU1</t>
+  </si>
+  <si>
+    <t>Super_man-2001</t>
+  </si>
+  <si>
+    <t>valid password</t>
+  </si>
+  <si>
+    <t>VP1</t>
+  </si>
+  <si>
+    <t>Krypton-was_2000</t>
+  </si>
+  <si>
+    <t>Negative Test Data</t>
+  </si>
+  <si>
+    <t>invalid username</t>
+  </si>
+  <si>
+    <t>requirement broken</t>
+  </si>
+  <si>
+    <t>IU1</t>
+  </si>
+  <si>
+    <t>Batman</t>
+  </si>
+  <si>
+    <t>IU2</t>
+  </si>
+  <si>
+    <t>Bane</t>
+  </si>
+  <si>
+    <t>IU3</t>
+  </si>
+  <si>
+    <t>wonder_woman_for_the_DC_theming</t>
+  </si>
+  <si>
+    <t>IU4</t>
+  </si>
+  <si>
+    <t>2face</t>
+  </si>
+  <si>
+    <t>IU5</t>
+  </si>
+  <si>
+    <t>joker!!!!!!?)</t>
+  </si>
+  <si>
+    <t>invalid password</t>
+  </si>
+  <si>
+    <t>IP1</t>
+  </si>
+  <si>
+    <t>b0Ts</t>
+  </si>
+  <si>
+    <t>IP2</t>
+  </si>
+  <si>
+    <t>AlfredIsTheBestButlerToExist111</t>
+  </si>
+  <si>
+    <t>IP3</t>
+  </si>
+  <si>
+    <t>3atman</t>
+  </si>
+  <si>
+    <t>IP4</t>
+  </si>
+  <si>
+    <t>A1fredIsTheBestButlerToExist!!</t>
+  </si>
+  <si>
+    <t>UR5, UR6</t>
+  </si>
+  <si>
+    <t>IP5</t>
+  </si>
+  <si>
+    <t>batman1</t>
+  </si>
+  <si>
+    <t>IP6</t>
+  </si>
+  <si>
+    <t>BATMAN1</t>
+  </si>
+  <si>
+    <t>IP7</t>
+  </si>
+  <si>
+    <t>Robin</t>
+  </si>
+  <si>
+    <t>Decision Table</t>
+  </si>
+  <si>
+    <t>Username</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>Expected Result</t>
+  </si>
+  <si>
+    <t>Account create successfully alert</t>
+  </si>
+  <si>
+    <t>Invalid username alert</t>
+  </si>
+  <si>
+    <t>Invalid password alert</t>
+  </si>
+  <si>
+    <t>Iamthenight1939</t>
+  </si>
+  <si>
+    <t>login success</t>
+  </si>
+  <si>
+    <t>Invalid Credentials alert</t>
+  </si>
+  <si>
+    <t>user state</t>
+  </si>
+  <si>
+    <t>expected result</t>
+  </si>
+  <si>
+    <t>logged in</t>
+  </si>
+  <si>
+    <t>logged out</t>
+  </si>
+  <si>
+    <t>can access home page directly</t>
+  </si>
+  <si>
+    <t>can not access home page directly</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -865,8 +1021,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -885,11 +1048,38 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
       <top/>
       <bottom/>
       <diagonal/>
@@ -898,7 +1088,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -925,6 +1115,51 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1020,63 +1255,57 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{1D12695F-9FC4-4685-A68A-139B4F574AF2}" name="Table210" displayName="Table210" ref="A1:B4" totalsRowShown="0" headerRowDxfId="15" dataDxfId="14">
+  <autoFilter ref="A1:B4" xr:uid="{1D12695F-9FC4-4685-A68A-139B4F574AF2}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{7A9A3850-4995-4F44-9EB0-B4715A60401A}" name="ID" dataDxfId="13"/>
+    <tableColumn id="2" xr3:uid="{683D9E57-68FD-47D3-918A-18C85478677D}" name="Security Requirement" dataDxfId="12"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{9EDF9F07-2176-4F4D-8482-8A0B579B8FE3}" name="Table312" displayName="Table312" ref="C1:D7" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+  <autoFilter ref="C1:D7" xr:uid="{9EDF9F07-2176-4F4D-8482-8A0B579B8FE3}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{0B4B587C-2987-47F9-A57C-DB73BF380CBF}" name="ID" dataDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{21CE179D-04E2-4D9A-B8DF-F348616A281F}" name="User Requirement" dataDxfId="8"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{7C9EDA58-99C2-4610-8B29-83D0FE4E6EFF}" name="Table414" displayName="Table414" ref="E1:F7" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
+  <autoFilter ref="E1:F7" xr:uid="{7C9EDA58-99C2-4610-8B29-83D0FE4E6EFF}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{FED4204E-184E-48A4-950E-2732B55B3358}" name="ID" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{5B55DAE8-DA35-40DF-8302-C5D3C4D96DB3}" name="Planet Requirement" dataDxfId="4"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{3CA5375E-FBF9-4C71-A96C-96E80144C074}" name="Table516" displayName="Table516" ref="G1:H8" totalsRowShown="0" headerRowDxfId="3" dataDxfId="2">
+  <autoFilter ref="G1:H8" xr:uid="{3CA5375E-FBF9-4C71-A96C-96E80144C074}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{8AF30F40-FA0B-4E71-B7B7-24A2D67C1960}" name="ID" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{2B6B577F-C2FB-46DB-B331-32DB697BFBF3}" name="Moon Requirement" dataDxfId="0"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{8C7A2EF1-1E3B-497A-963A-1E4B297B1AD8}" name="Table6" displayName="Table6" ref="A1:B15" totalsRowShown="0" headerRowDxfId="16">
-  <autoFilter ref="A1:B15" xr:uid="{8C7A2EF1-1E3B-497A-963A-1E4B297B1AD8}">
-    <filterColumn colId="0">
-      <filters>
-        <filter val="US1"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:B15" xr:uid="{8C7A2EF1-1E3B-497A-963A-1E4B297B1AD8}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{3E1D6F9B-CF49-4C23-A4F1-14FC88593279}" name="User Story"/>
     <tableColumn id="2" xr3:uid="{0AE99736-D95C-4721-996D-FB61185AF45C}" name="Requirement"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleDark5" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{CF32EC7D-69C5-4A93-8A2D-DC6765B2E759}" name="Table2" displayName="Table2" ref="A1:B4" totalsRowShown="0" headerRowDxfId="15" dataDxfId="14">
-  <autoFilter ref="A1:B4" xr:uid="{CF32EC7D-69C5-4A93-8A2D-DC6765B2E759}"/>
-  <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{516DE414-3CB5-42C3-B197-5FD33F813523}" name="ID" dataDxfId="13"/>
-    <tableColumn id="2" xr3:uid="{6D770425-64E8-434C-8D03-6414A09F53EC}" name="Security Requirement" dataDxfId="12"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{402AD37E-496A-4B82-BD5A-DDA158D6DA5D}" name="Table3" displayName="Table3" ref="A1:B7" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
-  <autoFilter ref="A1:B7" xr:uid="{402AD37E-496A-4B82-BD5A-DDA158D6DA5D}"/>
-  <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{77E4F913-7B38-4531-8FAA-D16B0FAAB464}" name="ID" dataDxfId="9"/>
-    <tableColumn id="2" xr3:uid="{85281BD9-33CE-4F6C-84B3-1E17141FF66A}" name="User Requirement" dataDxfId="8"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{79042BBB-0F12-4F67-90F0-C8062A2B8101}" name="Table4" displayName="Table4" ref="A1:B7" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
-  <autoFilter ref="A1:B7" xr:uid="{79042BBB-0F12-4F67-90F0-C8062A2B8101}"/>
-  <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{EC350D5A-6EAD-426C-A18A-35EC1B171BC1}" name="ID" dataDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{690F5785-7E7F-4D6A-8A10-FEEAAFDE3874}" name="Planet Requirement" dataDxfId="4"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{CB73B250-B846-4BAF-AF3B-5117DBBA4973}" name="Table5" displayName="Table5" ref="A1:B8" totalsRowShown="0" headerRowDxfId="3" dataDxfId="2">
-  <autoFilter ref="A1:B8" xr:uid="{CB73B250-B846-4BAF-AF3B-5117DBBA4973}"/>
-  <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{486EA324-F847-400D-80A5-266D5E36FC20}" name="ID" dataDxfId="1"/>
-    <tableColumn id="2" xr3:uid="{96D5BDBF-2AB3-4652-A2F0-CF69353F8D08}" name="Moon Requirement" dataDxfId="0"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -1467,97 +1696,208 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A2FE8F8-EFC1-44EB-82E1-9A97A755E2C6}">
-  <dimension ref="A1:B9"/>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD98B2F9-6983-475D-8F0E-27F4864D03DB}">
+  <dimension ref="A1:H8"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.28515625" customWidth="1"/>
-    <col min="2" max="2" width="27.42578125" customWidth="1"/>
+    <col min="1" max="1" width="27.5703125" customWidth="1"/>
+    <col min="2" max="2" width="27.7109375" customWidth="1"/>
+    <col min="3" max="3" width="27.28515625" customWidth="1"/>
+    <col min="4" max="4" width="27.7109375" customWidth="1"/>
+    <col min="5" max="7" width="27.28515625" customWidth="1"/>
+    <col min="8" max="8" width="27.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="H3" s="1" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="G4" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="H4" s="1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+    <row r="5" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="C5" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G5" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="H5" s="1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+    <row r="6" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="C6" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="G6" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="H6" s="1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+    <row r="7" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="C7" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="G7" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="H7" s="1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
+    <row r="8" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="G8" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="H8" s="1" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
+  <tableParts count="4">
     <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId4"/>
   </tableParts>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{751CFA12-0342-4856-9D1B-B622A006DBE5}">
   <dimension ref="A1:B22"/>
   <sheetViews>
@@ -1635,7 +1975,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="9" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -1643,7 +1983,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -1651,7 +1991,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -1659,7 +1999,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>9</v>
       </c>
@@ -1667,7 +2007,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>9</v>
       </c>
@@ -1675,7 +2015,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="14" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>9</v>
       </c>
@@ -1683,7 +2023,6 @@
         <v>55</v>
       </c>
     </row>
-    <row r="15" spans="1:2" hidden="1" x14ac:dyDescent="0.25"/>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>60</v>
@@ -1697,28 +2036,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D4693EB-185E-4567-AC0C-8312035BA2A5}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="27.42578125" customWidth="1"/>
-    <col min="2" max="2" width="27.5703125" customWidth="1"/>
-    <col min="3" max="3" width="28" customWidth="1"/>
-  </cols>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1DB7E24-71A0-45E8-B6FE-84B6B441D184}">
   <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A6" workbookViewId="0">
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
@@ -1903,6 +2225,564 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D4693EB-185E-4567-AC0C-8312035BA2A5}">
+  <dimension ref="A1:F36"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E30" sqref="E30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="31.140625" customWidth="1"/>
+    <col min="2" max="2" width="31.85546875" customWidth="1"/>
+    <col min="3" max="3" width="32.5703125" customWidth="1"/>
+    <col min="4" max="4" width="31.140625" customWidth="1"/>
+    <col min="5" max="5" width="31.85546875" customWidth="1"/>
+    <col min="6" max="6" width="32.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="13"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="15" t="s">
+        <v>95</v>
+      </c>
+      <c r="B2" s="15"/>
+      <c r="C2" s="16"/>
+      <c r="D2" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="17" t="s">
+        <v>96</v>
+      </c>
+      <c r="B3" s="17" t="s">
+        <v>97</v>
+      </c>
+      <c r="C3" s="18"/>
+      <c r="D3" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="E3" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="F3" s="2"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="19" t="s">
+        <v>98</v>
+      </c>
+      <c r="B4" s="19" t="s">
+        <v>99</v>
+      </c>
+      <c r="C4" s="18"/>
+      <c r="D4" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="F4" s="2"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="17" t="s">
+        <v>96</v>
+      </c>
+      <c r="B5" s="17" t="s">
+        <v>100</v>
+      </c>
+      <c r="C5" s="18"/>
+      <c r="D5" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="E5" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="F5" s="2"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="19" t="s">
+        <v>101</v>
+      </c>
+      <c r="B6" s="19" t="s">
+        <v>102</v>
+      </c>
+      <c r="C6" s="18"/>
+      <c r="D6" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="F6" s="2"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="20" t="s">
+        <v>103</v>
+      </c>
+      <c r="B7" s="20"/>
+      <c r="C7" s="21"/>
+      <c r="D7" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="17" t="s">
+        <v>96</v>
+      </c>
+      <c r="B8" s="17" t="s">
+        <v>104</v>
+      </c>
+      <c r="C8" s="22" t="s">
+        <v>105</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="E8" s="11" t="s">
+        <v>104</v>
+      </c>
+      <c r="F8" s="11" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="19" t="s">
+        <v>106</v>
+      </c>
+      <c r="B9" s="19" t="s">
+        <v>107</v>
+      </c>
+      <c r="C9" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="19" t="s">
+        <v>108</v>
+      </c>
+      <c r="B10" s="19" t="s">
+        <v>109</v>
+      </c>
+      <c r="C10" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="D10" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="E10" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="F10" s="11" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="19" t="s">
+        <v>110</v>
+      </c>
+      <c r="B11" s="19" t="s">
+        <v>111</v>
+      </c>
+      <c r="C11" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="19" t="s">
+        <v>112</v>
+      </c>
+      <c r="B12" s="19" t="s">
+        <v>113</v>
+      </c>
+      <c r="C12" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="D12" s="12" t="s">
+        <v>132</v>
+      </c>
+      <c r="E12" s="12"/>
+      <c r="F12" s="12"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="19" t="s">
+        <v>114</v>
+      </c>
+      <c r="B13" s="19" t="s">
+        <v>115</v>
+      </c>
+      <c r="C13" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="D13" s="11" t="s">
+        <v>133</v>
+      </c>
+      <c r="E13" s="11" t="s">
+        <v>134</v>
+      </c>
+      <c r="F13" s="11" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="17" t="s">
+        <v>96</v>
+      </c>
+      <c r="B14" s="17" t="s">
+        <v>116</v>
+      </c>
+      <c r="C14" s="22" t="s">
+        <v>105</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="19" t="s">
+        <v>117</v>
+      </c>
+      <c r="B15" s="19" t="s">
+        <v>118</v>
+      </c>
+      <c r="C15" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="19" t="s">
+        <v>119</v>
+      </c>
+      <c r="B16" s="19" t="s">
+        <v>120</v>
+      </c>
+      <c r="C16" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="19" t="s">
+        <v>121</v>
+      </c>
+      <c r="B17" s="19" t="s">
+        <v>122</v>
+      </c>
+      <c r="C17" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="19" t="s">
+        <v>123</v>
+      </c>
+      <c r="B18" s="19" t="s">
+        <v>124</v>
+      </c>
+      <c r="C18" s="18" t="s">
+        <v>125</v>
+      </c>
+      <c r="D18" s="11" t="s">
+        <v>142</v>
+      </c>
+      <c r="E18" s="11" t="s">
+        <v>143</v>
+      </c>
+      <c r="F18" s="2"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="19" t="s">
+        <v>126</v>
+      </c>
+      <c r="B19" s="19" t="s">
+        <v>127</v>
+      </c>
+      <c r="C19" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="F19" s="2"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="19" t="s">
+        <v>128</v>
+      </c>
+      <c r="B20" s="19" t="s">
+        <v>129</v>
+      </c>
+      <c r="C20" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="F20" s="2"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="19" t="s">
+        <v>130</v>
+      </c>
+      <c r="B21" s="19" t="s">
+        <v>131</v>
+      </c>
+      <c r="C21" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="23" t="s">
+        <v>132</v>
+      </c>
+      <c r="B22" s="23"/>
+      <c r="C22" s="24"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="17" t="s">
+        <v>133</v>
+      </c>
+      <c r="B23" s="17" t="s">
+        <v>134</v>
+      </c>
+      <c r="C23" s="22" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="19" t="s">
+        <v>98</v>
+      </c>
+      <c r="B24" s="19" t="s">
+        <v>101</v>
+      </c>
+      <c r="C24" s="18" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="19" t="s">
+        <v>106</v>
+      </c>
+      <c r="B25" s="19" t="s">
+        <v>101</v>
+      </c>
+      <c r="C25" s="18" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="19" t="s">
+        <v>108</v>
+      </c>
+      <c r="B26" s="19" t="s">
+        <v>101</v>
+      </c>
+      <c r="C26" s="18" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="19" t="s">
+        <v>110</v>
+      </c>
+      <c r="B27" s="19" t="s">
+        <v>101</v>
+      </c>
+      <c r="C27" s="18" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="19" t="s">
+        <v>112</v>
+      </c>
+      <c r="B28" s="19" t="s">
+        <v>101</v>
+      </c>
+      <c r="C28" s="18" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="19" t="s">
+        <v>114</v>
+      </c>
+      <c r="B29" s="19" t="s">
+        <v>101</v>
+      </c>
+      <c r="C29" s="18" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" s="19" t="s">
+        <v>98</v>
+      </c>
+      <c r="B30" s="19" t="s">
+        <v>117</v>
+      </c>
+      <c r="C30" s="18" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="19" t="s">
+        <v>98</v>
+      </c>
+      <c r="B31" s="19" t="s">
+        <v>119</v>
+      </c>
+      <c r="C31" s="18" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" s="19" t="s">
+        <v>98</v>
+      </c>
+      <c r="B32" s="19" t="s">
+        <v>121</v>
+      </c>
+      <c r="C32" s="18" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="19" t="s">
+        <v>98</v>
+      </c>
+      <c r="B33" s="19" t="s">
+        <v>123</v>
+      </c>
+      <c r="C33" s="18" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="19" t="s">
+        <v>98</v>
+      </c>
+      <c r="B34" s="19" t="s">
+        <v>126</v>
+      </c>
+      <c r="C34" s="18" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="19" t="s">
+        <v>98</v>
+      </c>
+      <c r="B35" s="19" t="s">
+        <v>128</v>
+      </c>
+      <c r="C35" s="18" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="19" t="s">
+        <v>98</v>
+      </c>
+      <c r="B36" s="19" t="s">
+        <v>130</v>
+      </c>
+      <c r="C36" s="18" t="s">
+        <v>138</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="8">
+    <mergeCell ref="D1:F1"/>
+    <mergeCell ref="D2:F2"/>
+    <mergeCell ref="D7:F7"/>
+    <mergeCell ref="D12:F12"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A7:C7"/>
+    <mergeCell ref="A22:C22"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E14EEDEC-6C50-4FA1-BB35-C40D70D716CC}">
   <dimension ref="A1:G29"/>
   <sheetViews>
@@ -2132,7 +3012,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9F5FABA-1ABC-4F95-8F7C-37C42F38162D}">
   <dimension ref="A1:D29"/>
   <sheetViews>
@@ -2354,230 +3234,4 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4F326BC-F067-41E8-847E-757ABB716A4D}">
-  <dimension ref="A1:B5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="27.5703125" customWidth="1"/>
-    <col min="2" max="2" width="27.7109375" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34D5955B-CBB4-4821-99BF-DB0B1EC1B1EA}">
-  <dimension ref="A1:B8"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:B7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="27.28515625" customWidth="1"/>
-    <col min="2" max="2" width="27.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46FBBBD4-BA32-4762-983D-1911FDD83C85}">
-  <dimension ref="A1:B9"/>
-  <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="2" width="27.28515625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
adding example feature files for project
</commit_message>
<xml_diff>
--- a/Project 1/Example RTM.xlsx
+++ b/Project 1/Example RTM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EricSuminski\Desktop\241209-JWA\Project 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{608E8196-9984-46DB-8747-F20D92353E3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15CEC7C9-5391-4C3C-8D08-63CC4EE617AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="3" xr2:uid="{F782749A-F44B-4770-ADC0-B107849E38C9}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="149">
   <si>
     <t>ID</t>
   </si>
@@ -632,6 +632,15 @@
     </r>
   </si>
   <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>Easy to associate code to acceptance criteria</t>
+  </si>
+  <si>
+    <t>Easy to associate code to acceptance criteria, but will involve writing out more code than the short option</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <b/>
@@ -641,6 +650,58 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
+      <t xml:space="preserve">When </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>the user provides one or more invalid credentials</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Then</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> the user should get a browser alert saying a credential is invalid</t>
+    </r>
+  </si>
+  <si>
+    <t>Requires a bit more work to associate acceptance criteria to code</t>
+  </si>
+  <si>
+    <t>negative</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>When</t>
     </r>
     <r>
@@ -651,6 +712,280 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
+      <t xml:space="preserve"> the user logs in</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Then</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> they should see their planets and moons</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Given</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> the user is not logged in</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>When</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> the user tries to directly access the home page</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Then</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> the user should be denied access</t>
+    </r>
+  </si>
+  <si>
+    <t>Positive Test Data</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>valid username</t>
+  </si>
+  <si>
+    <t>VU1</t>
+  </si>
+  <si>
+    <t>Super_man-2001</t>
+  </si>
+  <si>
+    <t>valid password</t>
+  </si>
+  <si>
+    <t>VP1</t>
+  </si>
+  <si>
+    <t>Krypton-was_2000</t>
+  </si>
+  <si>
+    <t>Negative Test Data</t>
+  </si>
+  <si>
+    <t>invalid username</t>
+  </si>
+  <si>
+    <t>requirement broken</t>
+  </si>
+  <si>
+    <t>IU1</t>
+  </si>
+  <si>
+    <t>Batman</t>
+  </si>
+  <si>
+    <t>IU2</t>
+  </si>
+  <si>
+    <t>Bane</t>
+  </si>
+  <si>
+    <t>IU3</t>
+  </si>
+  <si>
+    <t>wonder_woman_for_the_DC_theming</t>
+  </si>
+  <si>
+    <t>IU4</t>
+  </si>
+  <si>
+    <t>2face</t>
+  </si>
+  <si>
+    <t>IU5</t>
+  </si>
+  <si>
+    <t>joker!!!!!!?)</t>
+  </si>
+  <si>
+    <t>invalid password</t>
+  </si>
+  <si>
+    <t>IP1</t>
+  </si>
+  <si>
+    <t>b0Ts</t>
+  </si>
+  <si>
+    <t>IP2</t>
+  </si>
+  <si>
+    <t>AlfredIsTheBestButlerToExist111</t>
+  </si>
+  <si>
+    <t>IP3</t>
+  </si>
+  <si>
+    <t>3atman</t>
+  </si>
+  <si>
+    <t>IP4</t>
+  </si>
+  <si>
+    <t>A1fredIsTheBestButlerToExist!!</t>
+  </si>
+  <si>
+    <t>UR5, UR6</t>
+  </si>
+  <si>
+    <t>IP5</t>
+  </si>
+  <si>
+    <t>batman1</t>
+  </si>
+  <si>
+    <t>IP6</t>
+  </si>
+  <si>
+    <t>BATMAN1</t>
+  </si>
+  <si>
+    <t>IP7</t>
+  </si>
+  <si>
+    <t>Robin</t>
+  </si>
+  <si>
+    <t>Decision Table</t>
+  </si>
+  <si>
+    <t>Username</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>Expected Result</t>
+  </si>
+  <si>
+    <t>Account create successfully alert</t>
+  </si>
+  <si>
+    <t>Invalid username alert</t>
+  </si>
+  <si>
+    <t>Invalid password alert</t>
+  </si>
+  <si>
+    <t>Iamthenight1939</t>
+  </si>
+  <si>
+    <t>login success</t>
+  </si>
+  <si>
+    <t>Invalid Credentials alert</t>
+  </si>
+  <si>
+    <t>user state</t>
+  </si>
+  <si>
+    <t>expected result</t>
+  </si>
+  <si>
+    <t>logged in</t>
+  </si>
+  <si>
+    <t>logged out</t>
+  </si>
+  <si>
+    <t>can access home page directly</t>
+  </si>
+  <si>
+    <t>can not access home page directly</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>When</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
       <t xml:space="preserve"> the user provides username </t>
     </r>
     <r>
@@ -662,17 +997,8 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>"&lt;username input&gt;"</t>
-    </r>
-  </si>
-  <si>
-    <t>Notes</t>
-  </si>
-  <si>
-    <t>Easy to associate code to acceptance criteria</t>
-  </si>
-  <si>
-    <t>Easy to associate code to acceptance criteria, but will involve writing out more code than the short option</t>
+      <t>"&lt;username&gt;"</t>
+    </r>
   </si>
   <si>
     <r>
@@ -684,321 +1010,18 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">When </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>the user provides one or more invalid credentials</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Then</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> the user should get a browser alert saying a credential is invalid</t>
-    </r>
-  </si>
-  <si>
-    <t>Requires a bit more work to associate acceptance criteria to code</t>
-  </si>
-  <si>
-    <t>negative</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>When</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> the user logs in</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Then</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> they should see their planets and moons</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Given</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> the user is not logged in</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>When</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> the user tries to directly access the home page</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Then</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> the user should be denied access</t>
-    </r>
-  </si>
-  <si>
-    <t>Positive Test Data</t>
-  </si>
-  <si>
-    <t>id</t>
-  </si>
-  <si>
-    <t>valid username</t>
-  </si>
-  <si>
-    <t>VU1</t>
-  </si>
-  <si>
-    <t>Super_man-2001</t>
-  </si>
-  <si>
-    <t>valid password</t>
-  </si>
-  <si>
-    <t>VP1</t>
-  </si>
-  <si>
-    <t>Krypton-was_2000</t>
-  </si>
-  <si>
-    <t>Negative Test Data</t>
-  </si>
-  <si>
-    <t>invalid username</t>
-  </si>
-  <si>
-    <t>requirement broken</t>
-  </si>
-  <si>
-    <t>IU1</t>
-  </si>
-  <si>
-    <t>Batman</t>
-  </si>
-  <si>
-    <t>IU2</t>
-  </si>
-  <si>
-    <t>Bane</t>
-  </si>
-  <si>
-    <t>IU3</t>
-  </si>
-  <si>
-    <t>wonder_woman_for_the_DC_theming</t>
-  </si>
-  <si>
-    <t>IU4</t>
-  </si>
-  <si>
-    <t>2face</t>
-  </si>
-  <si>
-    <t>IU5</t>
-  </si>
-  <si>
-    <t>joker!!!!!!?)</t>
-  </si>
-  <si>
-    <t>invalid password</t>
-  </si>
-  <si>
-    <t>IP1</t>
-  </si>
-  <si>
-    <t>b0Ts</t>
-  </si>
-  <si>
-    <t>IP2</t>
-  </si>
-  <si>
-    <t>AlfredIsTheBestButlerToExist111</t>
-  </si>
-  <si>
-    <t>IP3</t>
-  </si>
-  <si>
-    <t>3atman</t>
-  </si>
-  <si>
-    <t>IP4</t>
-  </si>
-  <si>
-    <t>A1fredIsTheBestButlerToExist!!</t>
-  </si>
-  <si>
-    <t>UR5, UR6</t>
-  </si>
-  <si>
-    <t>IP5</t>
-  </si>
-  <si>
-    <t>batman1</t>
-  </si>
-  <si>
-    <t>IP6</t>
-  </si>
-  <si>
-    <t>BATMAN1</t>
-  </si>
-  <si>
-    <t>IP7</t>
-  </si>
-  <si>
-    <t>Robin</t>
-  </si>
-  <si>
-    <t>Decision Table</t>
-  </si>
-  <si>
-    <t>Username</t>
-  </si>
-  <si>
-    <t>Password</t>
-  </si>
-  <si>
-    <t>Expected Result</t>
-  </si>
-  <si>
-    <t>Account create successfully alert</t>
-  </si>
-  <si>
-    <t>Invalid username alert</t>
-  </si>
-  <si>
-    <t>Invalid password alert</t>
-  </si>
-  <si>
-    <t>Iamthenight1939</t>
-  </si>
-  <si>
-    <t>login success</t>
-  </si>
-  <si>
-    <t>Invalid Credentials alert</t>
-  </si>
-  <si>
-    <t>user state</t>
-  </si>
-  <si>
-    <t>expected result</t>
-  </si>
-  <si>
-    <t>logged in</t>
-  </si>
-  <si>
-    <t>logged out</t>
-  </si>
-  <si>
-    <t>can access home page directly</t>
-  </si>
-  <si>
-    <t>can not access home page directly</t>
+      <t>And</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> the user clicks the register link</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -1126,10 +1149,13 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1139,9 +1165,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1282,7 +1305,13 @@
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{8C7A2EF1-1E3B-497A-963A-1E4B297B1AD8}" name="Table6" displayName="Table6" ref="A1:B15" totalsRowShown="0" headerRowDxfId="0">
-  <autoFilter ref="A1:B15" xr:uid="{8C7A2EF1-1E3B-497A-963A-1E4B297B1AD8}"/>
+  <autoFilter ref="A1:B15" xr:uid="{8C7A2EF1-1E3B-497A-963A-1E4B297B1AD8}">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="US1"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{3E1D6F9B-CF49-4C23-A4F1-14FC88593279}" name="User Story"/>
     <tableColumn id="2" xr3:uid="{0AE99736-D95C-4721-996D-FB61185AF45C}" name="Requirement"/>
@@ -1611,7 +1640,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5:B6"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1672,8 +1701,9 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
@@ -1957,7 +1987,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -1965,7 +1995,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -1973,7 +2003,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -1981,7 +2011,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>9</v>
       </c>
@@ -1989,7 +2019,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>9</v>
       </c>
@@ -1997,7 +2027,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>9</v>
       </c>
@@ -2005,6 +2035,7 @@
         <v>55</v>
       </c>
     </row>
+    <row r="15" spans="1:2" hidden="1" x14ac:dyDescent="0.25"/>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>60</v>
@@ -2022,8 +2053,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1DB7E24-71A0-45E8-B6FE-84B6B441D184}">
   <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18:C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2045,7 +2076,7 @@
         <v>61</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -2067,7 +2098,7 @@
         <v>63</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -2121,7 +2152,7 @@
       <c r="A11" s="9"/>
       <c r="B11" s="8"/>
       <c r="C11" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -2135,7 +2166,7 @@
       <c r="A13" s="9"/>
       <c r="B13" s="8"/>
       <c r="C13" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -2160,37 +2191,37 @@
       <c r="A16" s="9"/>
       <c r="B16" s="10"/>
       <c r="C16" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="9"/>
       <c r="B17" s="10"/>
       <c r="C17" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="9"/>
       <c r="B18" s="11" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="9"/>
       <c r="B19" s="11"/>
       <c r="C19" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="9"/>
       <c r="B20" s="11"/>
       <c r="C20" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
   </sheetData>
@@ -2203,6 +2234,7 @@
     <mergeCell ref="B2:B7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2210,8 +2242,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D4693EB-185E-4567-AC0C-8312035BA2A5}">
   <dimension ref="A1:F36"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A22" sqref="A22:C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2225,140 +2257,140 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="13" t="s">
+      <c r="B1" s="15"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B2" s="12"/>
-      <c r="C2" s="16"/>
+      <c r="C2" s="17"/>
       <c r="D2" s="12" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E2" s="12"/>
       <c r="F2" s="12"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="B3" s="5" t="s">
         <v>96</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>97</v>
       </c>
       <c r="C3" s="6"/>
       <c r="D3" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="E3" s="5" t="s">
         <v>96</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>97</v>
       </c>
       <c r="F3" s="2"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>98</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>99</v>
       </c>
       <c r="C4" s="6"/>
       <c r="D4" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F4" s="2"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C5" s="6"/>
       <c r="D5" s="5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F5" s="2"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>101</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>102</v>
       </c>
       <c r="C6" s="6"/>
       <c r="D6" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F6" s="2"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B7" s="8"/>
-      <c r="C7" s="17"/>
+      <c r="C7" s="18"/>
       <c r="D7" s="8" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E7" s="8"/>
       <c r="F7" s="8"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B8" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="C8" s="7" t="s">
         <v>104</v>
       </c>
-      <c r="C8" s="7" t="s">
-        <v>105</v>
-      </c>
       <c r="D8" s="5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E8" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="F8" s="5" t="s">
         <v>104</v>
-      </c>
-      <c r="F8" s="5" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>106</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>107</v>
       </c>
       <c r="C9" s="6" t="s">
         <v>26</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F9" s="2" t="s">
         <v>18</v>
@@ -2366,39 +2398,39 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>108</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>109</v>
       </c>
       <c r="C10" s="6" t="s">
         <v>27</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>110</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>111</v>
       </c>
       <c r="C11" s="6" t="s">
         <v>27</v>
       </c>
       <c r="D11" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="E11" s="2" t="s">
         <v>117</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>118</v>
       </c>
       <c r="F11" s="2" t="s">
         <v>18</v>
@@ -2406,180 +2438,180 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="B12" s="2" t="s">
         <v>112</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>113</v>
       </c>
       <c r="C12" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="D12" s="14" t="s">
-        <v>132</v>
-      </c>
-      <c r="E12" s="14"/>
-      <c r="F12" s="14"/>
+      <c r="D12" s="13" t="s">
+        <v>131</v>
+      </c>
+      <c r="E12" s="13"/>
+      <c r="F12" s="13"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="B13" s="2" t="s">
         <v>114</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>115</v>
       </c>
       <c r="C13" s="6" t="s">
         <v>29</v>
       </c>
       <c r="D13" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="E13" s="5" t="s">
         <v>133</v>
       </c>
-      <c r="E13" s="5" t="s">
+      <c r="F13" s="5" t="s">
         <v>134</v>
-      </c>
-      <c r="F13" s="5" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="B15" s="2" t="s">
         <v>117</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>118</v>
       </c>
       <c r="C15" s="6" t="s">
         <v>27</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="B16" s="2" t="s">
         <v>119</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>120</v>
       </c>
       <c r="C16" s="6" t="s">
         <v>27</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="B17" s="2" t="s">
         <v>121</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>122</v>
       </c>
       <c r="C17" s="6" t="s">
         <v>28</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="B18" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="C18" s="6" t="s">
         <v>124</v>
       </c>
-      <c r="C18" s="6" t="s">
-        <v>125</v>
-      </c>
       <c r="D18" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="E18" s="5" t="s">
         <v>142</v>
-      </c>
-      <c r="E18" s="5" t="s">
-        <v>143</v>
       </c>
       <c r="F18" s="2"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="B19" s="2" t="s">
         <v>126</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>127</v>
       </c>
       <c r="C19" s="6" t="s">
         <v>30</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="F19" s="2"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="B20" s="2" t="s">
         <v>128</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>129</v>
       </c>
       <c r="C20" s="6" t="s">
         <v>30</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F20" s="2"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="B21" s="2" t="s">
         <v>130</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>131</v>
       </c>
       <c r="C21" s="6" t="s">
         <v>30</v>
@@ -2589,164 +2621,164 @@
       <c r="F21" s="2"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="14" t="s">
-        <v>132</v>
-      </c>
-      <c r="B22" s="14"/>
-      <c r="C22" s="18"/>
+      <c r="A22" s="13" t="s">
+        <v>131</v>
+      </c>
+      <c r="B22" s="13"/>
+      <c r="C22" s="14"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="B23" s="5" t="s">
         <v>133</v>
       </c>
-      <c r="B23" s="5" t="s">
+      <c r="C23" s="7" t="s">
         <v>134</v>
-      </c>
-      <c r="C23" s="7" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C32" s="6" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C34" s="6" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C35" s="6" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C36" s="6" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
   </sheetData>
@@ -2761,6 +2793,7 @@
     <mergeCell ref="A7:C7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2768,8 +2801,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E14EEDEC-6C50-4FA1-BB35-C40D70D716CC}">
   <dimension ref="A1:G29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2793,7 +2826,7 @@
         <v>61</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E1" s="1"/>
       <c r="G1" s="1"/>
@@ -2818,10 +2851,10 @@
       <c r="A3" s="9"/>
       <c r="B3" s="12"/>
       <c r="C3" s="1" t="s">
-        <v>63</v>
+        <v>148</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E3" s="1"/>
     </row>
@@ -2878,14 +2911,14 @@
       <c r="A10" s="9"/>
       <c r="B10" s="8"/>
       <c r="C10" s="1" t="s">
-        <v>63</v>
+        <v>148</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="9"/>
       <c r="B11" s="8"/>
       <c r="C11" s="1" t="s">
-        <v>82</v>
+        <v>147</v>
       </c>
       <c r="E11" s="1"/>
     </row>
@@ -2991,6 +3024,7 @@
     <mergeCell ref="B9:B15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -3022,7 +3056,7 @@
         <v>61</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="45" x14ac:dyDescent="0.25">
@@ -3036,7 +3070,7 @@
         <v>62</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
adding initial example test cases for User dao in planetarium
</commit_message>
<xml_diff>
--- a/Project 1/Example RTM.xlsx
+++ b/Project 1/Example RTM.xlsx
@@ -8,18 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EricSuminski\Desktop\241209-JWA\Project 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{065BDED8-BB9A-4ED8-B7F1-65CD0145B3D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7A3532F-0B67-4427-818A-2834C90C195B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="3" xr2:uid="{F782749A-F44B-4770-ADC0-B107849E38C9}"/>
+    <workbookView xWindow="-8445" yWindow="-16320" windowWidth="29040" windowHeight="15720" firstSheet="2" activeTab="5" xr2:uid="{F782749A-F44B-4770-ADC0-B107849E38C9}"/>
   </bookViews>
   <sheets>
     <sheet name="User Stories" sheetId="1" r:id="rId1"/>
     <sheet name="Requirements" sheetId="11" r:id="rId2"/>
     <sheet name="Mapping" sheetId="6" r:id="rId3"/>
     <sheet name="Acceptance Criteria General" sheetId="9" r:id="rId4"/>
-    <sheet name="Test Data" sheetId="10" r:id="rId5"/>
-    <sheet name="Acceptance Criteria Short" sheetId="7" r:id="rId6"/>
-    <sheet name="Acceptance Criteria Long" sheetId="8" r:id="rId7"/>
+    <sheet name="E2E Test Data" sheetId="10" r:id="rId5"/>
+    <sheet name="Repository Test Data" sheetId="12" r:id="rId6"/>
+    <sheet name="Acceptance Criteria Short" sheetId="7" r:id="rId7"/>
+    <sheet name="Acceptance Criteria Long" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -42,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="442" uniqueCount="159">
   <si>
     <t>ID</t>
   </si>
@@ -1022,6 +1023,36 @@
       </rPr>
       <t xml:space="preserve"> the user is logged in on the home page</t>
     </r>
+  </si>
+  <si>
+    <t>User Creation</t>
+  </si>
+  <si>
+    <t>valid user id</t>
+  </si>
+  <si>
+    <t>II1</t>
+  </si>
+  <si>
+    <t>invalid user id</t>
+  </si>
+  <si>
+    <t>User Id</t>
+  </si>
+  <si>
+    <t>VI1</t>
+  </si>
+  <si>
+    <t>User returned in Optional with Id set</t>
+  </si>
+  <si>
+    <t>*not required for MVP testing</t>
+  </si>
+  <si>
+    <t>Unhandled UserFail exception with message "Invalid username"</t>
+  </si>
+  <si>
+    <t>Unhandled UserFail exception with message "Invalid password"</t>
   </si>
 </sst>
 </file>
@@ -1111,7 +1142,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1133,6 +1164,12 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1166,6 +1203,10 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2046,7 +2087,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1DB7E24-71A0-45E8-B6FE-84B6B441D184}">
   <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+    <sheetView topLeftCell="A12" workbookViewId="0">
       <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
@@ -2073,10 +2114,10 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="14" t="s">
         <v>70</v>
       </c>
       <c r="C2" s="1" t="s">
@@ -2085,8 +2126,8 @@
       <c r="D2" s="4"/>
     </row>
     <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="9"/>
-      <c r="B3" s="12"/>
+      <c r="A3" s="11"/>
+      <c r="B3" s="14"/>
       <c r="C3" s="1" t="s">
         <v>63</v>
       </c>
@@ -2095,39 +2136,39 @@
       </c>
     </row>
     <row r="4" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="9"/>
-      <c r="B4" s="12"/>
+      <c r="A4" s="11"/>
+      <c r="B4" s="14"/>
       <c r="C4" s="1" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="9"/>
-      <c r="B5" s="12"/>
+      <c r="A5" s="11"/>
+      <c r="B5" s="14"/>
       <c r="C5" s="1" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="9"/>
-      <c r="B6" s="12"/>
+      <c r="A6" s="11"/>
+      <c r="B6" s="14"/>
       <c r="C6" s="1" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="9"/>
-      <c r="B7" s="12"/>
+      <c r="A7" s="11"/>
+      <c r="B7" s="14"/>
       <c r="C7" s="1" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="9"/>
+      <c r="A8" s="11"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="9"/>
-      <c r="B9" s="8" t="s">
+      <c r="A9" s="11"/>
+      <c r="B9" s="10" t="s">
         <v>71</v>
       </c>
       <c r="C9" s="1" t="s">
@@ -2135,45 +2176,45 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="9"/>
-      <c r="B10" s="8"/>
+      <c r="A10" s="11"/>
+      <c r="B10" s="10"/>
       <c r="C10" s="1" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="9"/>
-      <c r="B11" s="8"/>
+      <c r="A11" s="11"/>
+      <c r="B11" s="10"/>
       <c r="C11" s="1" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="9"/>
-      <c r="B12" s="8"/>
+      <c r="A12" s="11"/>
+      <c r="B12" s="10"/>
       <c r="C12" s="1" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="9"/>
-      <c r="B13" s="8"/>
+      <c r="A13" s="11"/>
+      <c r="B13" s="10"/>
       <c r="C13" s="1" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="9"/>
-      <c r="B14" s="8"/>
+      <c r="A14" s="11"/>
+      <c r="B14" s="10"/>
       <c r="C14" s="1" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="9" t="s">
+      <c r="A15" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="B15" s="10" t="s">
+      <c r="B15" s="12" t="s">
         <v>70</v>
       </c>
       <c r="C15" s="1" t="s">
@@ -2181,20 +2222,20 @@
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="9"/>
-      <c r="B16" s="10"/>
+      <c r="A16" s="11"/>
+      <c r="B16" s="12"/>
       <c r="C16" s="1"/>
     </row>
     <row r="17" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="9"/>
-      <c r="B17" s="10"/>
+      <c r="A17" s="11"/>
+      <c r="B17" s="12"/>
       <c r="C17" s="1" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="9"/>
-      <c r="B18" s="11" t="s">
+      <c r="A18" s="11"/>
+      <c r="B18" s="13" t="s">
         <v>88</v>
       </c>
       <c r="C18" s="1" t="s">
@@ -2202,15 +2243,15 @@
       </c>
     </row>
     <row r="19" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A19" s="9"/>
-      <c r="B19" s="11"/>
+      <c r="A19" s="11"/>
+      <c r="B19" s="13"/>
       <c r="C19" s="1" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="9"/>
-      <c r="B20" s="11"/>
+      <c r="A20" s="11"/>
+      <c r="B20" s="13"/>
       <c r="C20" s="1" t="s">
         <v>92</v>
       </c>
@@ -2234,7 +2275,7 @@
   <dimension ref="A1:F36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A22" sqref="A22:C36"/>
+      <selection activeCell="A2" sqref="A2:C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2248,28 +2289,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="15" t="s">
+      <c r="B1" s="17"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="14" t="s">
         <v>93</v>
       </c>
-      <c r="B2" s="12"/>
-      <c r="C2" s="17"/>
-      <c r="D2" s="12" t="s">
+      <c r="B2" s="14"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="14" t="s">
         <v>93</v>
       </c>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
@@ -2336,16 +2377,16 @@
       <c r="F6" s="2"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="8" t="s">
+      <c r="A7" s="10" t="s">
         <v>101</v>
       </c>
-      <c r="B7" s="8"/>
-      <c r="C7" s="18"/>
-      <c r="D7" s="8" t="s">
+      <c r="B7" s="10"/>
+      <c r="C7" s="20"/>
+      <c r="D7" s="10" t="s">
         <v>101</v>
       </c>
-      <c r="E7" s="8"/>
-      <c r="F7" s="8"/>
+      <c r="E7" s="10"/>
+      <c r="F7" s="10"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
@@ -2437,11 +2478,11 @@
       <c r="C12" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="D12" s="13" t="s">
+      <c r="D12" s="15" t="s">
         <v>130</v>
       </c>
-      <c r="E12" s="13"/>
-      <c r="F12" s="13"/>
+      <c r="E12" s="15"/>
+      <c r="F12" s="15"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
@@ -2612,11 +2653,11 @@
       <c r="F21" s="2"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="13" t="s">
+      <c r="A22" s="15" t="s">
         <v>130</v>
       </c>
-      <c r="B22" s="13"/>
-      <c r="C22" s="14"/>
+      <c r="B22" s="15"/>
+      <c r="C22" s="16"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
@@ -2789,6 +2830,489 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8BD42B9-EB2E-468F-9F50-2ECA73E20FAE}">
+  <dimension ref="A1:D40"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="J31" sqref="J31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="31.140625" customWidth="1"/>
+    <col min="2" max="2" width="31.85546875" customWidth="1"/>
+    <col min="3" max="3" width="32.5703125" customWidth="1"/>
+    <col min="4" max="4" width="27.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="17" t="s">
+        <v>149</v>
+      </c>
+      <c r="B1" s="17"/>
+      <c r="C1" s="18"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="14" t="s">
+        <v>93</v>
+      </c>
+      <c r="B2" s="14"/>
+      <c r="C2" s="19"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="C3" s="6"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="C4" s="6"/>
+      <c r="D4" s="2"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="C5" s="6"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="C6" s="6"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="21" t="s">
+        <v>94</v>
+      </c>
+      <c r="B7" s="21" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>154</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="B9" s="10"/>
+      <c r="C9" s="20"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="C24" s="7" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="B25" s="2">
+        <v>1</v>
+      </c>
+      <c r="C25" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="D25" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="8" t="s">
+        <v>130</v>
+      </c>
+      <c r="B26" s="8"/>
+      <c r="C26" s="9"/>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="D27" s="7" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="D28" s="6" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="D29" s="6" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="D30" s="6" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="D31" s="6" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="D32" s="6" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="D33" s="6" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="D34" s="6" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="D35" s="6" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="D36" s="6" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A37" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="D37" s="6" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A38" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="D38" s="6" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A39" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="D39" s="6" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A40" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="D40" s="6" t="s">
+        <v>158</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A9:C9"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E14EEDEC-6C50-4FA1-BB35-C40D70D716CC}">
   <dimension ref="A1:G29"/>
   <sheetViews>
@@ -2823,10 +3347,10 @@
       <c r="G1" s="1"/>
     </row>
     <row r="2" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="14" t="s">
         <v>70</v>
       </c>
       <c r="C2" s="1" t="s">
@@ -2839,8 +3363,8 @@
       <c r="G2" s="4"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="9"/>
-      <c r="B3" s="12"/>
+      <c r="A3" s="11"/>
+      <c r="B3" s="14"/>
       <c r="C3" s="1" t="s">
         <v>147</v>
       </c>
@@ -2850,48 +3374,48 @@
       <c r="E3" s="1"/>
     </row>
     <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="9"/>
-      <c r="B4" s="12"/>
+      <c r="A4" s="11"/>
+      <c r="B4" s="14"/>
       <c r="C4" s="1" t="s">
         <v>64</v>
       </c>
       <c r="E4" s="1"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="9"/>
-      <c r="B5" s="12"/>
+      <c r="A5" s="11"/>
+      <c r="B5" s="14"/>
       <c r="C5" s="1" t="s">
         <v>65</v>
       </c>
       <c r="E5" s="1"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="9"/>
-      <c r="B6" s="12"/>
+      <c r="A6" s="11"/>
+      <c r="B6" s="14"/>
       <c r="C6" s="1" t="s">
         <v>66</v>
       </c>
       <c r="E6" s="1"/>
     </row>
     <row r="7" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="9"/>
-      <c r="B7" s="12"/>
+      <c r="A7" s="11"/>
+      <c r="B7" s="14"/>
       <c r="C7" s="1" t="s">
         <v>67</v>
       </c>
       <c r="E7" s="1"/>
     </row>
     <row r="8" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="9"/>
-      <c r="B8" s="12"/>
+      <c r="A8" s="11"/>
+      <c r="B8" s="14"/>
       <c r="C8" s="1" t="s">
         <v>68</v>
       </c>
       <c r="E8" s="1"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="9"/>
-      <c r="B9" s="8" t="s">
+      <c r="A9" s="11"/>
+      <c r="B9" s="10" t="s">
         <v>71</v>
       </c>
       <c r="C9" s="1" t="s">
@@ -2899,47 +3423,47 @@
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="9"/>
-      <c r="B10" s="8"/>
+      <c r="A10" s="11"/>
+      <c r="B10" s="10"/>
       <c r="C10" s="1" t="s">
         <v>147</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="9"/>
-      <c r="B11" s="8"/>
+      <c r="A11" s="11"/>
+      <c r="B11" s="10"/>
       <c r="C11" s="1" t="s">
         <v>146</v>
       </c>
       <c r="E11" s="1"/>
     </row>
     <row r="12" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="9"/>
-      <c r="B12" s="8"/>
+      <c r="A12" s="11"/>
+      <c r="B12" s="10"/>
       <c r="C12" s="1" t="s">
         <v>80</v>
       </c>
       <c r="E12" s="1"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="9"/>
-      <c r="B13" s="8"/>
+      <c r="A13" s="11"/>
+      <c r="B13" s="10"/>
       <c r="C13" s="1" t="s">
         <v>66</v>
       </c>
       <c r="E13" s="1"/>
     </row>
     <row r="14" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="9"/>
-      <c r="B14" s="8"/>
+      <c r="A14" s="11"/>
+      <c r="B14" s="10"/>
       <c r="C14" s="1" t="s">
         <v>81</v>
       </c>
       <c r="E14" s="1"/>
     </row>
     <row r="15" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="9"/>
-      <c r="B15" s="8"/>
+      <c r="A15" s="11"/>
+      <c r="B15" s="10"/>
       <c r="C15" s="1" t="s">
         <v>75</v>
       </c>
@@ -3019,7 +3543,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9F5FABA-1ABC-4F95-8F7C-37C42F38162D}">
   <dimension ref="A1:D29"/>
   <sheetViews>
@@ -3054,7 +3578,7 @@
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="14" t="s">
         <v>70</v>
       </c>
       <c r="C2" s="1" t="s">
@@ -3065,43 +3589,43 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B3" s="12"/>
+      <c r="B3" s="14"/>
       <c r="C3" s="1" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="B4" s="12"/>
+      <c r="B4" s="14"/>
       <c r="C4" s="1" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B5" s="12"/>
+      <c r="B5" s="14"/>
       <c r="C5" s="1" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B6" s="12"/>
+      <c r="B6" s="14"/>
       <c r="C6" s="1" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="B7" s="12"/>
+      <c r="B7" s="14"/>
       <c r="C7" s="1" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="B8" s="12"/>
+      <c r="B8" s="14"/>
       <c r="C8" s="1" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B9" s="8" t="s">
+      <c r="B9" s="10" t="s">
         <v>71</v>
       </c>
       <c r="C9" s="1" t="s">
@@ -3109,43 +3633,43 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B10" s="8"/>
+      <c r="B10" s="10"/>
       <c r="C10" s="1" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="B11" s="8"/>
+      <c r="B11" s="10"/>
       <c r="C11" s="1" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B12" s="8"/>
+      <c r="B12" s="10"/>
       <c r="C12" s="1" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B13" s="8"/>
+      <c r="B13" s="10"/>
       <c r="C13" s="1" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="B14" s="8"/>
+      <c r="B14" s="10"/>
       <c r="C14" s="1" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="B15" s="8"/>
+      <c r="B15" s="10"/>
       <c r="C15" s="1" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B16" s="8" t="s">
+      <c r="B16" s="10" t="s">
         <v>71</v>
       </c>
       <c r="C16" s="1" t="s">
@@ -3153,43 +3677,43 @@
       </c>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B17" s="8"/>
+      <c r="B17" s="10"/>
       <c r="C17" s="1" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="18" spans="2:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="B18" s="8"/>
+      <c r="B18" s="10"/>
       <c r="C18" s="1" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="19" spans="2:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="B19" s="8"/>
+      <c r="B19" s="10"/>
       <c r="C19" s="1" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B20" s="8"/>
+      <c r="B20" s="10"/>
       <c r="C20" s="1" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="21" spans="2:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="B21" s="8"/>
+      <c r="B21" s="10"/>
       <c r="C21" s="1" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="22" spans="2:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="B22" s="8"/>
+      <c r="B22" s="10"/>
       <c r="C22" s="1" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="23" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B23" s="8" t="s">
+      <c r="B23" s="10" t="s">
         <v>71</v>
       </c>
       <c r="C23" s="1" t="s">
@@ -3197,37 +3721,37 @@
       </c>
     </row>
     <row r="24" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B24" s="8"/>
+      <c r="B24" s="10"/>
       <c r="C24" s="1" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="25" spans="2:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="B25" s="8"/>
+      <c r="B25" s="10"/>
       <c r="C25" s="1" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="26" spans="2:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="B26" s="8"/>
+      <c r="B26" s="10"/>
       <c r="C26" s="1" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="27" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B27" s="8"/>
+      <c r="B27" s="10"/>
       <c r="C27" s="1" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="28" spans="2:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="B28" s="8"/>
+      <c r="B28" s="10"/>
       <c r="C28" s="1" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="29" spans="2:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="B29" s="8"/>
+      <c r="B29" s="10"/>
       <c r="C29" s="1" t="s">
         <v>75</v>
       </c>

</xml_diff>

<commit_message>
adding negative integration tests
</commit_message>
<xml_diff>
--- a/Project 1/Example RTM.xlsx
+++ b/Project 1/Example RTM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EricSuminski\Desktop\241209-JWA\Project 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7A3532F-0B67-4427-818A-2834C90C195B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87A07B98-AB76-4D4C-8E0F-4F6159368835}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-8445" yWindow="-16320" windowWidth="29040" windowHeight="15720" firstSheet="2" activeTab="5" xr2:uid="{F782749A-F44B-4770-ADC0-B107849E38C9}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" firstSheet="2" activeTab="5" xr2:uid="{F782749A-F44B-4770-ADC0-B107849E38C9}"/>
   </bookViews>
   <sheets>
     <sheet name="User Stories" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="442" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="458" uniqueCount="168">
   <si>
     <t>ID</t>
   </si>
@@ -1025,9 +1025,6 @@
     </r>
   </si>
   <si>
-    <t>User Creation</t>
-  </si>
-  <si>
     <t>valid user id</t>
   </si>
   <si>
@@ -1053,6 +1050,36 @@
   </si>
   <si>
     <t>Unhandled UserFail exception with message "Invalid password"</t>
+  </si>
+  <si>
+    <t>User Data</t>
+  </si>
+  <si>
+    <t>valid current username</t>
+  </si>
+  <si>
+    <t>valid current password</t>
+  </si>
+  <si>
+    <t>valid current user id</t>
+  </si>
+  <si>
+    <t>Decision Table: user creation</t>
+  </si>
+  <si>
+    <t>Decision Table: authentication</t>
+  </si>
+  <si>
+    <t>user id</t>
+  </si>
+  <si>
+    <t>username</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>Unhandled UserFail exception with message "Invalid credentials"</t>
   </si>
 </sst>
 </file>
@@ -1142,7 +1169,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1171,6 +1198,7 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1204,8 +1232,10 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2114,10 +2144,10 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="15" t="s">
         <v>70</v>
       </c>
       <c r="C2" s="1" t="s">
@@ -2126,8 +2156,8 @@
       <c r="D2" s="4"/>
     </row>
     <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="11"/>
-      <c r="B3" s="14"/>
+      <c r="A3" s="12"/>
+      <c r="B3" s="15"/>
       <c r="C3" s="1" t="s">
         <v>63</v>
       </c>
@@ -2136,39 +2166,39 @@
       </c>
     </row>
     <row r="4" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="11"/>
-      <c r="B4" s="14"/>
+      <c r="A4" s="12"/>
+      <c r="B4" s="15"/>
       <c r="C4" s="1" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="11"/>
-      <c r="B5" s="14"/>
+      <c r="A5" s="12"/>
+      <c r="B5" s="15"/>
       <c r="C5" s="1" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="11"/>
-      <c r="B6" s="14"/>
+      <c r="A6" s="12"/>
+      <c r="B6" s="15"/>
       <c r="C6" s="1" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="11"/>
-      <c r="B7" s="14"/>
+      <c r="A7" s="12"/>
+      <c r="B7" s="15"/>
       <c r="C7" s="1" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="11"/>
+      <c r="A8" s="12"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="11"/>
-      <c r="B9" s="10" t="s">
+      <c r="A9" s="12"/>
+      <c r="B9" s="11" t="s">
         <v>71</v>
       </c>
       <c r="C9" s="1" t="s">
@@ -2176,45 +2206,45 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="11"/>
-      <c r="B10" s="10"/>
+      <c r="A10" s="12"/>
+      <c r="B10" s="11"/>
       <c r="C10" s="1" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="11"/>
-      <c r="B11" s="10"/>
+      <c r="A11" s="12"/>
+      <c r="B11" s="11"/>
       <c r="C11" s="1" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="11"/>
-      <c r="B12" s="10"/>
+      <c r="A12" s="12"/>
+      <c r="B12" s="11"/>
       <c r="C12" s="1" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="11"/>
-      <c r="B13" s="10"/>
+      <c r="A13" s="12"/>
+      <c r="B13" s="11"/>
       <c r="C13" s="1" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="11"/>
-      <c r="B14" s="10"/>
+      <c r="A14" s="12"/>
+      <c r="B14" s="11"/>
       <c r="C14" s="1" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="11" t="s">
+      <c r="A15" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="B15" s="12" t="s">
+      <c r="B15" s="13" t="s">
         <v>70</v>
       </c>
       <c r="C15" s="1" t="s">
@@ -2222,20 +2252,20 @@
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="11"/>
-      <c r="B16" s="12"/>
+      <c r="A16" s="12"/>
+      <c r="B16" s="13"/>
       <c r="C16" s="1"/>
     </row>
     <row r="17" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="11"/>
-      <c r="B17" s="12"/>
+      <c r="A17" s="12"/>
+      <c r="B17" s="13"/>
       <c r="C17" s="1" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="11"/>
-      <c r="B18" s="13" t="s">
+      <c r="A18" s="12"/>
+      <c r="B18" s="14" t="s">
         <v>88</v>
       </c>
       <c r="C18" s="1" t="s">
@@ -2243,15 +2273,15 @@
       </c>
     </row>
     <row r="19" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A19" s="11"/>
-      <c r="B19" s="13"/>
+      <c r="A19" s="12"/>
+      <c r="B19" s="14"/>
       <c r="C19" s="1" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="11"/>
-      <c r="B20" s="13"/>
+      <c r="A20" s="12"/>
+      <c r="B20" s="14"/>
       <c r="C20" s="1" t="s">
         <v>92</v>
       </c>
@@ -2289,28 +2319,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="17" t="s">
+      <c r="B1" s="18"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="15" t="s">
         <v>93</v>
       </c>
-      <c r="B2" s="14"/>
-      <c r="C2" s="19"/>
-      <c r="D2" s="14" t="s">
+      <c r="B2" s="15"/>
+      <c r="C2" s="20"/>
+      <c r="D2" s="15" t="s">
         <v>93</v>
       </c>
-      <c r="E2" s="14"/>
-      <c r="F2" s="14"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
@@ -2377,16 +2407,16 @@
       <c r="F6" s="2"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="10" t="s">
+      <c r="A7" s="11" t="s">
         <v>101</v>
       </c>
-      <c r="B7" s="10"/>
-      <c r="C7" s="20"/>
-      <c r="D7" s="10" t="s">
+      <c r="B7" s="11"/>
+      <c r="C7" s="21"/>
+      <c r="D7" s="11" t="s">
         <v>101</v>
       </c>
-      <c r="E7" s="10"/>
-      <c r="F7" s="10"/>
+      <c r="E7" s="11"/>
+      <c r="F7" s="11"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
@@ -2478,11 +2508,11 @@
       <c r="C12" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="D12" s="15" t="s">
+      <c r="D12" s="16" t="s">
         <v>130</v>
       </c>
-      <c r="E12" s="15"/>
-      <c r="F12" s="15"/>
+      <c r="E12" s="16"/>
+      <c r="F12" s="16"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
@@ -2653,11 +2683,11 @@
       <c r="F21" s="2"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="15" t="s">
+      <c r="A22" s="16" t="s">
         <v>130</v>
       </c>
-      <c r="B22" s="15"/>
-      <c r="C22" s="16"/>
+      <c r="B22" s="16"/>
+      <c r="C22" s="17"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
@@ -2831,10 +2861,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8BD42B9-EB2E-468F-9F50-2ECA73E20FAE}">
-  <dimension ref="A1:D40"/>
+  <dimension ref="A1:D44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="J31" sqref="J31"/>
+    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
+      <selection activeCell="F41" sqref="F41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2846,18 +2876,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="17" t="s">
-        <v>149</v>
-      </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="18"/>
+      <c r="A1" s="18" t="s">
+        <v>158</v>
+      </c>
+      <c r="B1" s="18"/>
+      <c r="C1" s="19"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="15" t="s">
         <v>93</v>
       </c>
-      <c r="B2" s="14"/>
-      <c r="C2" s="19"/>
+      <c r="B2" s="15"/>
+      <c r="C2" s="20"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
@@ -2866,7 +2896,9 @@
       <c r="B3" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="C3" s="6"/>
+      <c r="C3" s="7" t="s">
+        <v>159</v>
+      </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
@@ -2875,7 +2907,9 @@
       <c r="B4" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="C4" s="6"/>
+      <c r="C4" s="6" t="s">
+        <v>105</v>
+      </c>
       <c r="D4" s="2"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -2885,7 +2919,9 @@
       <c r="B5" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="C5" s="6"/>
+      <c r="C5" s="7" t="s">
+        <v>160</v>
+      </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
@@ -2894,30 +2930,38 @@
       <c r="B6" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="C6" s="6"/>
+      <c r="C6" s="6" t="s">
+        <v>137</v>
+      </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="21" t="s">
+      <c r="A7" s="10" t="s">
         <v>94</v>
       </c>
-      <c r="B7" s="21" t="s">
-        <v>150</v>
+      <c r="B7" s="10" t="s">
+        <v>149</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>161</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B8">
         <v>0</v>
       </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="10" t="s">
+      <c r="A9" s="11" t="s">
         <v>101</v>
       </c>
-      <c r="B9" s="10"/>
-      <c r="C9" s="20"/>
+      <c r="B9" s="11"/>
+      <c r="C9" s="21"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
@@ -3078,7 +3122,7 @@
         <v>94</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C24" s="7" t="s">
         <v>103</v>
@@ -3086,28 +3130,28 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B25" s="2">
         <v>1</v>
       </c>
-      <c r="C25" s="22" t="s">
+      <c r="C25" s="6" t="s">
         <v>17</v>
       </c>
       <c r="D25" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="8" t="s">
-        <v>130</v>
+        <v>162</v>
       </c>
       <c r="B26" s="8"/>
       <c r="C26" s="9"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B27" s="5" t="s">
         <v>131</v>
@@ -3121,7 +3165,7 @@
     </row>
     <row r="28" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>96</v>
@@ -3130,12 +3174,12 @@
         <v>99</v>
       </c>
       <c r="D28" s="6" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>104</v>
@@ -3144,12 +3188,12 @@
         <v>99</v>
       </c>
       <c r="D29" s="6" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>106</v>
@@ -3158,12 +3202,12 @@
         <v>99</v>
       </c>
       <c r="D30" s="6" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B31" s="2" t="s">
         <v>108</v>
@@ -3172,12 +3216,12 @@
         <v>99</v>
       </c>
       <c r="D31" s="6" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B32" s="2" t="s">
         <v>110</v>
@@ -3186,12 +3230,12 @@
         <v>99</v>
       </c>
       <c r="D32" s="6" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B33" s="2" t="s">
         <v>112</v>
@@ -3200,12 +3244,12 @@
         <v>99</v>
       </c>
       <c r="D33" s="6" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B34" s="2" t="s">
         <v>96</v>
@@ -3214,12 +3258,12 @@
         <v>115</v>
       </c>
       <c r="D34" s="6" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B35" s="2" t="s">
         <v>96</v>
@@ -3228,12 +3272,12 @@
         <v>117</v>
       </c>
       <c r="D35" s="6" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B36" s="2" t="s">
         <v>96</v>
@@ -3242,12 +3286,12 @@
         <v>119</v>
       </c>
       <c r="D36" s="6" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B37" s="2" t="s">
         <v>96</v>
@@ -3256,12 +3300,12 @@
         <v>121</v>
       </c>
       <c r="D37" s="6" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B38" s="2" t="s">
         <v>96</v>
@@ -3270,12 +3314,12 @@
         <v>124</v>
       </c>
       <c r="D38" s="6" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B39" s="2" t="s">
         <v>96</v>
@@ -3284,12 +3328,12 @@
         <v>126</v>
       </c>
       <c r="D39" s="6" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B40" s="2" t="s">
         <v>96</v>
@@ -3298,7 +3342,57 @@
         <v>128</v>
       </c>
       <c r="D40" s="6" t="s">
-        <v>158</v>
+        <v>157</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="8" t="s">
+        <v>163</v>
+      </c>
+      <c r="B41" s="8"/>
+      <c r="C41" s="9"/>
+      <c r="D41" s="9"/>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="5" t="s">
+        <v>164</v>
+      </c>
+      <c r="B42" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="C42" s="23" t="s">
+        <v>166</v>
+      </c>
+      <c r="D42" s="23" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>0</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="C43" s="22" t="s">
+        <v>129</v>
+      </c>
+      <c r="D43" s="6" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>0</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="C44" s="22" t="s">
+        <v>137</v>
+      </c>
+      <c r="D44" s="6" t="s">
+        <v>167</v>
       </c>
     </row>
   </sheetData>
@@ -3347,10 +3441,10 @@
       <c r="G1" s="1"/>
     </row>
     <row r="2" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="15" t="s">
         <v>70</v>
       </c>
       <c r="C2" s="1" t="s">
@@ -3363,8 +3457,8 @@
       <c r="G2" s="4"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="11"/>
-      <c r="B3" s="14"/>
+      <c r="A3" s="12"/>
+      <c r="B3" s="15"/>
       <c r="C3" s="1" t="s">
         <v>147</v>
       </c>
@@ -3374,48 +3468,48 @@
       <c r="E3" s="1"/>
     </row>
     <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="11"/>
-      <c r="B4" s="14"/>
+      <c r="A4" s="12"/>
+      <c r="B4" s="15"/>
       <c r="C4" s="1" t="s">
         <v>64</v>
       </c>
       <c r="E4" s="1"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="11"/>
-      <c r="B5" s="14"/>
+      <c r="A5" s="12"/>
+      <c r="B5" s="15"/>
       <c r="C5" s="1" t="s">
         <v>65</v>
       </c>
       <c r="E5" s="1"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="11"/>
-      <c r="B6" s="14"/>
+      <c r="A6" s="12"/>
+      <c r="B6" s="15"/>
       <c r="C6" s="1" t="s">
         <v>66</v>
       </c>
       <c r="E6" s="1"/>
     </row>
     <row r="7" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="11"/>
-      <c r="B7" s="14"/>
+      <c r="A7" s="12"/>
+      <c r="B7" s="15"/>
       <c r="C7" s="1" t="s">
         <v>67</v>
       </c>
       <c r="E7" s="1"/>
     </row>
     <row r="8" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="11"/>
-      <c r="B8" s="14"/>
+      <c r="A8" s="12"/>
+      <c r="B8" s="15"/>
       <c r="C8" s="1" t="s">
         <v>68</v>
       </c>
       <c r="E8" s="1"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="11"/>
-      <c r="B9" s="10" t="s">
+      <c r="A9" s="12"/>
+      <c r="B9" s="11" t="s">
         <v>71</v>
       </c>
       <c r="C9" s="1" t="s">
@@ -3423,47 +3517,47 @@
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="11"/>
-      <c r="B10" s="10"/>
+      <c r="A10" s="12"/>
+      <c r="B10" s="11"/>
       <c r="C10" s="1" t="s">
         <v>147</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="11"/>
-      <c r="B11" s="10"/>
+      <c r="A11" s="12"/>
+      <c r="B11" s="11"/>
       <c r="C11" s="1" t="s">
         <v>146</v>
       </c>
       <c r="E11" s="1"/>
     </row>
     <row r="12" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="11"/>
-      <c r="B12" s="10"/>
+      <c r="A12" s="12"/>
+      <c r="B12" s="11"/>
       <c r="C12" s="1" t="s">
         <v>80</v>
       </c>
       <c r="E12" s="1"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="11"/>
-      <c r="B13" s="10"/>
+      <c r="A13" s="12"/>
+      <c r="B13" s="11"/>
       <c r="C13" s="1" t="s">
         <v>66</v>
       </c>
       <c r="E13" s="1"/>
     </row>
     <row r="14" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="11"/>
-      <c r="B14" s="10"/>
+      <c r="A14" s="12"/>
+      <c r="B14" s="11"/>
       <c r="C14" s="1" t="s">
         <v>81</v>
       </c>
       <c r="E14" s="1"/>
     </row>
     <row r="15" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="11"/>
-      <c r="B15" s="10"/>
+      <c r="A15" s="12"/>
+      <c r="B15" s="11"/>
       <c r="C15" s="1" t="s">
         <v>75</v>
       </c>
@@ -3578,7 +3672,7 @@
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="15" t="s">
         <v>70</v>
       </c>
       <c r="C2" s="1" t="s">
@@ -3589,43 +3683,43 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B3" s="14"/>
+      <c r="B3" s="15"/>
       <c r="C3" s="1" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="B4" s="14"/>
+      <c r="B4" s="15"/>
       <c r="C4" s="1" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B5" s="14"/>
+      <c r="B5" s="15"/>
       <c r="C5" s="1" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B6" s="14"/>
+      <c r="B6" s="15"/>
       <c r="C6" s="1" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="B7" s="14"/>
+      <c r="B7" s="15"/>
       <c r="C7" s="1" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="B8" s="14"/>
+      <c r="B8" s="15"/>
       <c r="C8" s="1" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B9" s="10" t="s">
+      <c r="B9" s="11" t="s">
         <v>71</v>
       </c>
       <c r="C9" s="1" t="s">
@@ -3633,43 +3727,43 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B10" s="10"/>
+      <c r="B10" s="11"/>
       <c r="C10" s="1" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="B11" s="10"/>
+      <c r="B11" s="11"/>
       <c r="C11" s="1" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B12" s="10"/>
+      <c r="B12" s="11"/>
       <c r="C12" s="1" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B13" s="10"/>
+      <c r="B13" s="11"/>
       <c r="C13" s="1" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="B14" s="10"/>
+      <c r="B14" s="11"/>
       <c r="C14" s="1" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="B15" s="10"/>
+      <c r="B15" s="11"/>
       <c r="C15" s="1" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B16" s="10" t="s">
+      <c r="B16" s="11" t="s">
         <v>71</v>
       </c>
       <c r="C16" s="1" t="s">
@@ -3677,43 +3771,43 @@
       </c>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B17" s="10"/>
+      <c r="B17" s="11"/>
       <c r="C17" s="1" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="18" spans="2:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="B18" s="10"/>
+      <c r="B18" s="11"/>
       <c r="C18" s="1" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="19" spans="2:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="B19" s="10"/>
+      <c r="B19" s="11"/>
       <c r="C19" s="1" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B20" s="10"/>
+      <c r="B20" s="11"/>
       <c r="C20" s="1" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="21" spans="2:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="B21" s="10"/>
+      <c r="B21" s="11"/>
       <c r="C21" s="1" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="22" spans="2:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="B22" s="10"/>
+      <c r="B22" s="11"/>
       <c r="C22" s="1" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="23" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B23" s="10" t="s">
+      <c r="B23" s="11" t="s">
         <v>71</v>
       </c>
       <c r="C23" s="1" t="s">
@@ -3721,37 +3815,37 @@
       </c>
     </row>
     <row r="24" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B24" s="10"/>
+      <c r="B24" s="11"/>
       <c r="C24" s="1" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="25" spans="2:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="B25" s="10"/>
+      <c r="B25" s="11"/>
       <c r="C25" s="1" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="26" spans="2:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="B26" s="10"/>
+      <c r="B26" s="11"/>
       <c r="C26" s="1" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="27" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B27" s="10"/>
+      <c r="B27" s="11"/>
       <c r="C27" s="1" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="28" spans="2:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="B28" s="10"/>
+      <c r="B28" s="11"/>
       <c r="C28" s="1" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="29" spans="2:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="B29" s="10"/>
+      <c r="B29" s="11"/>
       <c r="C29" s="1" t="s">
         <v>75</v>
       </c>

</xml_diff>